<commit_message>
Update Excel for the depth calculation of a pool
</commit_message>
<xml_diff>
--- a/teaser/examples/2021-03-24_Hüllflächen_Zonen_Shells_of_Zones.xlsx
+++ b/teaser/examples/2021-03-24_Hüllflächen_Zonen_Shells_of_Zones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmi\.conda\envs\py37\lib\site-packages\teaser\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\TEASER\teaser\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2719D74-7376-48E4-A793-A65FFACED2AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D9C528-F533-4D5B-96C7-E5436187B1ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hüllflächen, Himmelsricht." sheetId="1" r:id="rId1"/>
@@ -2035,6 +2035,69 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2047,95 +2110,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2184,6 +2184,579 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="Textfeld 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75605227-E849-45E4-95C6-77E002F8DC3A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="33775650" y="6629400"/>
+              <a:ext cx="4298950" cy="889000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+                <a:t>Für Vario und Mehrzweckbecken wird dei Tiefe anteilig für die unterschiedlichen Zonen mit unterschiedlichen Tiefen berechnet:</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑎</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>= </m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝐴</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>&lt;1,35</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>∗</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑎</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>&lt;1,35</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>+  </m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝐴</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>≥1,35</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>∗</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑎</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>≥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>1,35</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝐴</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑔𝑒𝑠</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="de-DE" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="Textfeld 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75605227-E849-45E4-95C6-77E002F8DC3A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="33775650" y="6629400"/>
+              <a:ext cx="4298950" cy="889000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+                <a:t>Für Vario und Mehrzweckbecken wird dei Tiefe anteilig für die unterschiedlichen Zonen mit unterschiedlichen Tiefen berechnet:</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑎=  (𝐴_(&lt;1,35)∗𝑎_(&lt;1,35)+  𝐴_(≥1,35)∗𝑎_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>≥</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>1,35))/𝐴_𝑔𝑒𝑠 </a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2525,8 +3098,8 @@
   </sheetPr>
   <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2564,25 +3137,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="165" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
-      <c r="I1" s="188"/>
-      <c r="J1" s="188"/>
-      <c r="K1" s="188"/>
-      <c r="L1" s="188"/>
-      <c r="M1" s="188"/>
-      <c r="N1" s="188"/>
-      <c r="O1" s="188"/>
-      <c r="P1" s="188"/>
-      <c r="Q1" s="188"/>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="40"/>
@@ -2605,42 +3178,42 @@
     </row>
     <row r="3" spans="1:31" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="26"/>
-      <c r="B3" s="181" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="182"/>
-      <c r="D3" s="183" t="s">
+      <c r="B3" s="184" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="177"/>
+      <c r="D3" s="173" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="184"/>
-      <c r="F3" s="185" t="s">
+      <c r="E3" s="175"/>
+      <c r="F3" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="182"/>
-      <c r="H3" s="191" t="s">
+      <c r="G3" s="177"/>
+      <c r="H3" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="184"/>
-      <c r="J3" s="185" t="s">
+      <c r="I3" s="175"/>
+      <c r="J3" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="182"/>
-      <c r="L3" s="189" t="s">
+      <c r="K3" s="177"/>
+      <c r="L3" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="190"/>
-      <c r="N3" s="189" t="s">
+      <c r="M3" s="172"/>
+      <c r="N3" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="190"/>
-      <c r="P3" s="183" t="s">
+      <c r="O3" s="172"/>
+      <c r="P3" s="173" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="183"/>
-      <c r="S3" s="165" t="s">
+      <c r="Q3" s="173"/>
+      <c r="S3" s="186" t="s">
         <v>46</v>
       </c>
-      <c r="T3" s="166"/>
+      <c r="T3" s="187"/>
       <c r="U3" s="163" t="s">
         <v>58</v>
       </c>
@@ -2676,40 +3249,40 @@
       <c r="A4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="186" t="s">
+      <c r="B4" s="170" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="170"/>
+      <c r="C4" s="185"/>
       <c r="D4" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="170"/>
+      <c r="E4" s="185"/>
       <c r="F4" s="169" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="170"/>
+      <c r="G4" s="185"/>
       <c r="H4" s="169" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="170"/>
-      <c r="J4" s="171" t="s">
+      <c r="I4" s="185"/>
+      <c r="J4" s="190" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="172"/>
-      <c r="L4" s="173" t="s">
+      <c r="K4" s="191"/>
+      <c r="L4" s="167" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="174"/>
-      <c r="N4" s="173" t="s">
+      <c r="M4" s="168"/>
+      <c r="N4" s="167" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="174"/>
+      <c r="O4" s="168"/>
       <c r="P4" s="169" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="186"/>
-      <c r="S4" s="167"/>
-      <c r="T4" s="168"/>
+      <c r="Q4" s="170"/>
+      <c r="S4" s="188"/>
+      <c r="T4" s="189"/>
       <c r="U4" s="48" t="s">
         <v>47</v>
       </c>
@@ -2742,7 +3315,7 @@
       </c>
     </row>
     <row r="5" spans="1:31" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="175" t="s">
+      <c r="A5" s="178" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2833,7 +3406,7 @@
       </c>
     </row>
     <row r="6" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="176"/>
+      <c r="A6" s="179"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -2922,7 +3495,7 @@
       <c r="AE6" s="132"/>
     </row>
     <row r="7" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="176"/>
+      <c r="A7" s="179"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -3007,7 +3580,7 @@
       </c>
     </row>
     <row r="8" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="177"/>
+      <c r="A8" s="180"/>
       <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3095,7 +3668,7 @@
       </c>
     </row>
     <row r="9" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="178" t="s">
+      <c r="A9" s="181" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -3188,7 +3761,7 @@
       </c>
     </row>
     <row r="10" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="179"/>
+      <c r="A10" s="182"/>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -3276,7 +3849,7 @@
       <c r="AE10" s="47"/>
     </row>
     <row r="11" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="179"/>
+      <c r="A11" s="182"/>
       <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
@@ -3359,7 +3932,7 @@
       <c r="AE11" s="47"/>
     </row>
     <row r="12" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="180"/>
+      <c r="A12" s="183"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -4341,6 +4914,19 @@
     <row r="30" spans="1:32" ht="46.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="P4:Q4"/>
@@ -4349,19 +4935,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
   </mergeCells>
   <conditionalFormatting sqref="B23">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
@@ -4398,7 +4971,8 @@
   <ignoredErrors>
     <ignoredError sqref="G16 E16 C16 V8" formula="1"/>
   </ignoredErrors>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4407,7 +4981,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -4427,12 +5001,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="197" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
       <c r="E1" s="44"/>
       <c r="F1" s="14"/>
       <c r="G1" s="55"/>
@@ -4506,7 +5080,7 @@
       <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="197" t="s">
+      <c r="A4" s="198" t="s">
         <v>69</v>
       </c>
       <c r="B4" s="46"/>
@@ -4529,21 +5103,21 @@
       <c r="I4" s="62">
         <v>0.77584580000000003</v>
       </c>
-      <c r="J4" s="194" t="s">
+      <c r="J4" s="196" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="194" t="s">
+      <c r="K4" s="196" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="194" t="s">
+      <c r="L4" s="196" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="194" t="s">
+      <c r="M4" s="196" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="194"/>
+      <c r="A5" s="196"/>
       <c r="B5" s="46"/>
       <c r="C5" s="46"/>
       <c r="D5" s="12">
@@ -4564,13 +5138,13 @@
       <c r="I5" s="62">
         <v>1.45</v>
       </c>
-      <c r="J5" s="194"/>
-      <c r="K5" s="194"/>
-      <c r="L5" s="194"/>
-      <c r="M5" s="194"/>
+      <c r="J5" s="196"/>
+      <c r="K5" s="196"/>
+      <c r="L5" s="196"/>
+      <c r="M5" s="196"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="194"/>
+      <c r="A6" s="196"/>
       <c r="B6" s="46"/>
       <c r="C6" s="46"/>
       <c r="D6" s="12">
@@ -4591,13 +5165,13 @@
       <c r="I6" s="62">
         <v>10</v>
       </c>
-      <c r="J6" s="194"/>
-      <c r="K6" s="194"/>
-      <c r="L6" s="194"/>
-      <c r="M6" s="194"/>
+      <c r="J6" s="196"/>
+      <c r="K6" s="196"/>
+      <c r="L6" s="196"/>
+      <c r="M6" s="196"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="194"/>
+      <c r="A7" s="196"/>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
       <c r="D7" s="12">
@@ -4618,25 +5192,25 @@
       <c r="I7" s="62">
         <v>1</v>
       </c>
-      <c r="J7" s="194"/>
-      <c r="K7" s="194"/>
-      <c r="L7" s="194"/>
-      <c r="M7" s="194"/>
+      <c r="J7" s="196"/>
+      <c r="K7" s="196"/>
+      <c r="L7" s="196"/>
+      <c r="M7" s="196"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="194"/>
+      <c r="A8" s="196"/>
       <c r="B8" s="46"/>
       <c r="C8" s="46"/>
       <c r="D8" s="12">
         <v>4</v>
       </c>
-      <c r="J8" s="194"/>
-      <c r="K8" s="194"/>
-      <c r="L8" s="194"/>
-      <c r="M8" s="194"/>
+      <c r="J8" s="196"/>
+      <c r="K8" s="196"/>
+      <c r="L8" s="196"/>
+      <c r="M8" s="196"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="195"/>
+      <c r="A9" s="194"/>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="13">
@@ -4644,10 +5218,10 @@
       </c>
       <c r="H9" s="55"/>
       <c r="I9" s="55"/>
-      <c r="J9" s="195"/>
-      <c r="K9" s="195"/>
-      <c r="L9" s="195"/>
-      <c r="M9" s="195"/>
+      <c r="J9" s="194"/>
+      <c r="K9" s="194"/>
+      <c r="L9" s="194"/>
+      <c r="M9" s="194"/>
     </row>
     <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="192" t="s">
@@ -4679,11 +5253,11 @@
       <c r="M10" s="192" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="198" t="s">
+      <c r="N10" s="195" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="198"/>
-      <c r="P10" s="198"/>
+      <c r="O10" s="195"/>
+      <c r="P10" s="195"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="193"/>
@@ -4705,9 +5279,9 @@
       <c r="K11" s="193"/>
       <c r="L11" s="193"/>
       <c r="M11" s="193"/>
-      <c r="N11" s="198"/>
-      <c r="O11" s="198"/>
-      <c r="P11" s="198"/>
+      <c r="N11" s="195"/>
+      <c r="O11" s="195"/>
+      <c r="P11" s="195"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="193"/>
@@ -4723,13 +5297,13 @@
         <v>30</v>
       </c>
       <c r="I12" s="12"/>
-      <c r="J12" s="194"/>
-      <c r="K12" s="194"/>
-      <c r="L12" s="194"/>
-      <c r="M12" s="194"/>
-      <c r="N12" s="198"/>
-      <c r="O12" s="198"/>
-      <c r="P12" s="198"/>
+      <c r="J12" s="196"/>
+      <c r="K12" s="196"/>
+      <c r="L12" s="196"/>
+      <c r="M12" s="196"/>
+      <c r="N12" s="195"/>
+      <c r="O12" s="195"/>
+      <c r="P12" s="195"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="193"/>
@@ -4743,13 +5317,13 @@
       <c r="G13" s="53"/>
       <c r="H13" s="53"/>
       <c r="I13" s="12"/>
-      <c r="J13" s="194"/>
-      <c r="K13" s="194"/>
-      <c r="L13" s="194"/>
-      <c r="M13" s="194"/>
-      <c r="N13" s="198"/>
-      <c r="O13" s="198"/>
-      <c r="P13" s="198"/>
+      <c r="J13" s="196"/>
+      <c r="K13" s="196"/>
+      <c r="L13" s="196"/>
+      <c r="M13" s="196"/>
+      <c r="N13" s="195"/>
+      <c r="O13" s="195"/>
+      <c r="P13" s="195"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="193"/>
@@ -4763,16 +5337,16 @@
       <c r="G14" s="53"/>
       <c r="H14" s="53"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="194"/>
-      <c r="K14" s="194"/>
-      <c r="L14" s="194"/>
-      <c r="M14" s="194"/>
-      <c r="N14" s="198"/>
-      <c r="O14" s="198"/>
-      <c r="P14" s="198"/>
+      <c r="J14" s="196"/>
+      <c r="K14" s="196"/>
+      <c r="L14" s="196"/>
+      <c r="M14" s="196"/>
+      <c r="N14" s="195"/>
+      <c r="O14" s="195"/>
+      <c r="P14" s="195"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="195"/>
+      <c r="A15" s="194"/>
       <c r="B15" s="44"/>
       <c r="C15" s="55"/>
       <c r="D15" s="13">
@@ -4783,13 +5357,13 @@
       <c r="G15" s="53"/>
       <c r="H15" s="55"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="195"/>
-      <c r="K15" s="195"/>
-      <c r="L15" s="195"/>
-      <c r="M15" s="195"/>
-      <c r="N15" s="198"/>
-      <c r="O15" s="198"/>
-      <c r="P15" s="198"/>
+      <c r="J15" s="194"/>
+      <c r="K15" s="194"/>
+      <c r="L15" s="194"/>
+      <c r="M15" s="194"/>
+      <c r="N15" s="195"/>
+      <c r="O15" s="195"/>
+      <c r="P15" s="195"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="192" t="s">
@@ -4958,10 +5532,10 @@
       <c r="I21" s="55">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J21" s="194"/>
-      <c r="K21" s="194"/>
-      <c r="L21" s="194"/>
-      <c r="M21" s="194"/>
+      <c r="J21" s="196"/>
+      <c r="K21" s="196"/>
+      <c r="L21" s="196"/>
+      <c r="M21" s="196"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="192" t="s">
@@ -5109,7 +5683,7 @@
       <c r="M26" s="193"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="195"/>
+      <c r="A27" s="194"/>
       <c r="B27" s="44"/>
       <c r="C27" s="55"/>
       <c r="D27" s="13">
@@ -5130,10 +5704,10 @@
       <c r="I27" s="55">
         <v>1.38</v>
       </c>
-      <c r="J27" s="195"/>
-      <c r="K27" s="195"/>
-      <c r="L27" s="195"/>
-      <c r="M27" s="195"/>
+      <c r="J27" s="194"/>
+      <c r="K27" s="194"/>
+      <c r="L27" s="194"/>
+      <c r="M27" s="194"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="192" t="s">
@@ -5223,7 +5797,7 @@
       <c r="M32" s="193"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="195"/>
+      <c r="A33" s="194"/>
       <c r="B33" s="79"/>
       <c r="C33" s="79"/>
       <c r="D33" s="13">
@@ -5234,10 +5808,10 @@
       <c r="G33" s="79"/>
       <c r="H33" s="79"/>
       <c r="I33" s="79"/>
-      <c r="J33" s="195"/>
-      <c r="K33" s="195"/>
-      <c r="L33" s="195"/>
-      <c r="M33" s="195"/>
+      <c r="J33" s="194"/>
+      <c r="K33" s="194"/>
+      <c r="L33" s="194"/>
+      <c r="M33" s="194"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="192" t="s">
@@ -5327,7 +5901,7 @@
       <c r="M38" s="193"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="195"/>
+      <c r="A39" s="194"/>
       <c r="B39" s="79"/>
       <c r="C39" s="79"/>
       <c r="D39" s="13">
@@ -5338,10 +5912,10 @@
       <c r="G39" s="79"/>
       <c r="H39" s="79"/>
       <c r="I39" s="79"/>
-      <c r="J39" s="195"/>
-      <c r="K39" s="195"/>
-      <c r="L39" s="195"/>
-      <c r="M39" s="195"/>
+      <c r="J39" s="194"/>
+      <c r="K39" s="194"/>
+      <c r="L39" s="194"/>
+      <c r="M39" s="194"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="52" t="s">
@@ -5488,7 +6062,7 @@
       <c r="M46" s="193"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" s="195"/>
+      <c r="A47" s="194"/>
       <c r="B47" s="152"/>
       <c r="C47" s="152"/>
       <c r="D47" s="13">
@@ -5499,28 +6073,26 @@
       <c r="G47" s="152"/>
       <c r="H47" s="152"/>
       <c r="I47" s="152"/>
-      <c r="J47" s="195"/>
-      <c r="K47" s="195"/>
-      <c r="L47" s="195"/>
-      <c r="M47" s="195"/>
+      <c r="J47" s="194"/>
+      <c r="K47" s="194"/>
+      <c r="L47" s="194"/>
+      <c r="M47" s="194"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="J42:J47"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="M42:M47"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="J34:J39"/>
-    <mergeCell ref="K34:K39"/>
-    <mergeCell ref="L34:L39"/>
-    <mergeCell ref="M34:M39"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="J28:J33"/>
-    <mergeCell ref="K28:K33"/>
-    <mergeCell ref="L28:L33"/>
-    <mergeCell ref="M28:M33"/>
+    <mergeCell ref="L16:L21"/>
+    <mergeCell ref="M16:M21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="J22:J27"/>
+    <mergeCell ref="K22:K27"/>
+    <mergeCell ref="L22:L27"/>
+    <mergeCell ref="M22:M27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="K16:K21"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="J16:J21"/>
     <mergeCell ref="N10:P15"/>
     <mergeCell ref="M10:M15"/>
     <mergeCell ref="J4:J9"/>
@@ -5530,19 +6102,21 @@
     <mergeCell ref="J10:J15"/>
     <mergeCell ref="K10:K15"/>
     <mergeCell ref="L10:L15"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="K16:K21"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="J16:J21"/>
-    <mergeCell ref="L16:L21"/>
-    <mergeCell ref="M16:M21"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="J22:J27"/>
-    <mergeCell ref="K22:K27"/>
-    <mergeCell ref="L22:L27"/>
-    <mergeCell ref="M22:M27"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="J28:J33"/>
+    <mergeCell ref="K28:K33"/>
+    <mergeCell ref="L28:L33"/>
+    <mergeCell ref="M28:M33"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="J34:J39"/>
+    <mergeCell ref="K34:K39"/>
+    <mergeCell ref="L34:L39"/>
+    <mergeCell ref="M34:M39"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="J42:J47"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="M42:M47"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Parameters in SwimmingPool Calculation and Excel
</commit_message>
<xml_diff>
--- a/teaser/examples/2021-03-24_Hüllflächen_Zonen_Shells_of_Zones.xlsx
+++ b/teaser/examples/2021-03-24_Hüllflächen_Zonen_Shells_of_Zones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\TEASER\teaser\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D9C528-F533-4D5B-96C7-E5436187B1ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70A6A2B-90C6-40DE-98B3-CA9F9E7014E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hüllflächen, Himmelsricht." sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="137">
   <si>
     <t>Zone 1</t>
   </si>
@@ -663,9 +663,6 @@
     <t>Freiformbecken4</t>
   </si>
   <si>
-    <t>Salzwasser</t>
-  </si>
-  <si>
     <t>Süßwasser</t>
   </si>
   <si>
@@ -693,9 +690,6 @@
     <t>Filtertyp</t>
   </si>
   <si>
-    <t>Aktivkohlefilter mit Ozon</t>
-  </si>
-  <si>
     <t>Quarzkiesfilter</t>
   </si>
   <si>
@@ -709,6 +703,32 @@
   </si>
   <si>
     <t>Aufbereitungsvolumenstrom Nachts</t>
+  </si>
+  <si>
+    <t>offener Saugfilter</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Gemittelte Tiefe!</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2035,107 +2055,107 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2184,579 +2204,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="Textfeld 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75605227-E849-45E4-95C6-77E002F8DC3A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="33775650" y="6629400"/>
-              <a:ext cx="4298950" cy="889000"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="20000"/>
-                <a:lumOff val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln w="9525" cmpd="sng">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" baseline="0"/>
-                <a:t>Für Vario und Mehrzweckbecken wird dei Tiefe anteilig für die unterschiedlichen Zonen mit unterschiedlichen Tiefen berechnet:</a:t>
-              </a:r>
-            </a:p>
-            <a:p>
-              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                <a:lnSpc>
-                  <a:spcPct val="100000"/>
-                </a:lnSpc>
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-                <a:buClrTx/>
-                <a:buSzTx/>
-                <a:buFontTx/>
-                <a:buNone/>
-                <a:tabLst/>
-                <a:defRPr/>
-              </a:pPr>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>𝑎</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>= </m:t>
-                    </m:r>
-                    <m:f>
-                      <m:fPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="dk1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="+mn-ea"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:fPr>
-                      <m:num>
-                        <m:sSub>
-                          <m:sSubPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSubPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝐴</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sub>
-                            <m:r>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>&lt;1,35</m:t>
-                            </m:r>
-                          </m:sub>
-                        </m:sSub>
-                        <m:r>
-                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="dk1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="+mn-ea"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t>∗</m:t>
-                        </m:r>
-                        <m:sSub>
-                          <m:sSubPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSubPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝑎</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sub>
-                            <m:r>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>&lt;1,35</m:t>
-                            </m:r>
-                          </m:sub>
-                        </m:sSub>
-                        <m:r>
-                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="dk1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="+mn-ea"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t>+  </m:t>
-                        </m:r>
-                        <m:sSub>
-                          <m:sSubPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSubPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝐴</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sub>
-                            <m:r>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>≥1,35</m:t>
-                            </m:r>
-                          </m:sub>
-                        </m:sSub>
-                        <m:r>
-                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="dk1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="+mn-ea"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t>∗</m:t>
-                        </m:r>
-                        <m:sSub>
-                          <m:sSubPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSubPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝑎</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sub>
-                            <m:r>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>≥</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>1,35</m:t>
-                            </m:r>
-                          </m:sub>
-                        </m:sSub>
-                      </m:num>
-                      <m:den>
-                        <m:sSub>
-                          <m:sSubPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSubPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝐴</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sub>
-                            <m:r>
-                              <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="dk1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝑔𝑒𝑠</m:t>
-                            </m:r>
-                          </m:sub>
-                        </m:sSub>
-                      </m:den>
-                    </m:f>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="de-DE" sz="1100"/>
-            </a:p>
-            <a:p>
-              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                <a:lnSpc>
-                  <a:spcPct val="100000"/>
-                </a:lnSpc>
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-                <a:buClrTx/>
-                <a:buSzTx/>
-                <a:buFontTx/>
-                <a:buNone/>
-                <a:tabLst/>
-                <a:defRPr/>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="Textfeld 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75605227-E849-45E4-95C6-77E002F8DC3A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="33775650" y="6629400"/>
-              <a:ext cx="4298950" cy="889000"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="20000"/>
-                <a:lumOff val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln w="9525" cmpd="sng">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" baseline="0"/>
-                <a:t>Für Vario und Mehrzweckbecken wird dei Tiefe anteilig für die unterschiedlichen Zonen mit unterschiedlichen Tiefen berechnet:</a:t>
-              </a:r>
-            </a:p>
-            <a:p>
-              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                <a:lnSpc>
-                  <a:spcPct val="100000"/>
-                </a:lnSpc>
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-                <a:buClrTx/>
-                <a:buSzTx/>
-                <a:buFontTx/>
-                <a:buNone/>
-                <a:tabLst/>
-                <a:defRPr/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝑎=  (𝐴_(&lt;1,35)∗𝑎_(&lt;1,35)+  𝐴_(≥1,35)∗𝑎_(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>≥</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>1,35))/𝐴_𝑔𝑒𝑠 </a:t>
-              </a:r>
-              <a:endParaRPr lang="de-DE" sz="1100"/>
-            </a:p>
-            <a:p>
-              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                <a:lnSpc>
-                  <a:spcPct val="100000"/>
-                </a:lnSpc>
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-                <a:buClrTx/>
-                <a:buSzTx/>
-                <a:buFontTx/>
-                <a:buNone/>
-                <a:tabLst/>
-                <a:defRPr/>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3098,8 +2545,8 @@
   </sheetPr>
   <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE14" sqref="AE14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3137,25 +2584,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
+      <c r="K1" s="188"/>
+      <c r="L1" s="188"/>
+      <c r="M1" s="188"/>
+      <c r="N1" s="188"/>
+      <c r="O1" s="188"/>
+      <c r="P1" s="188"/>
+      <c r="Q1" s="188"/>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="40"/>
@@ -3178,42 +2625,42 @@
     </row>
     <row r="3" spans="1:31" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="26"/>
-      <c r="B3" s="184" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="177"/>
-      <c r="D3" s="173" t="s">
+      <c r="B3" s="181" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="182"/>
+      <c r="D3" s="183" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="175"/>
-      <c r="F3" s="176" t="s">
+      <c r="E3" s="184"/>
+      <c r="F3" s="185" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="177"/>
-      <c r="H3" s="174" t="s">
+      <c r="G3" s="182"/>
+      <c r="H3" s="191" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="175"/>
-      <c r="J3" s="176" t="s">
+      <c r="I3" s="184"/>
+      <c r="J3" s="185" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="177"/>
-      <c r="L3" s="171" t="s">
+      <c r="K3" s="182"/>
+      <c r="L3" s="189" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="172"/>
-      <c r="N3" s="171" t="s">
+      <c r="M3" s="190"/>
+      <c r="N3" s="189" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="172"/>
-      <c r="P3" s="173" t="s">
+      <c r="O3" s="190"/>
+      <c r="P3" s="183" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="173"/>
-      <c r="S3" s="186" t="s">
+      <c r="Q3" s="183"/>
+      <c r="S3" s="165" t="s">
         <v>46</v>
       </c>
-      <c r="T3" s="187"/>
+      <c r="T3" s="166"/>
       <c r="U3" s="163" t="s">
         <v>58</v>
       </c>
@@ -3249,40 +2696,40 @@
       <c r="A4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="186" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="185"/>
+      <c r="C4" s="170"/>
       <c r="D4" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="185"/>
+      <c r="E4" s="170"/>
       <c r="F4" s="169" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="185"/>
+      <c r="G4" s="170"/>
       <c r="H4" s="169" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="185"/>
-      <c r="J4" s="190" t="s">
+      <c r="I4" s="170"/>
+      <c r="J4" s="171" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="191"/>
-      <c r="L4" s="167" t="s">
+      <c r="K4" s="172"/>
+      <c r="L4" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="168"/>
-      <c r="N4" s="167" t="s">
+      <c r="M4" s="174"/>
+      <c r="N4" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="168"/>
+      <c r="O4" s="174"/>
       <c r="P4" s="169" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="170"/>
-      <c r="S4" s="188"/>
-      <c r="T4" s="189"/>
+      <c r="Q4" s="186"/>
+      <c r="S4" s="167"/>
+      <c r="T4" s="168"/>
       <c r="U4" s="48" t="s">
         <v>47</v>
       </c>
@@ -3315,7 +2762,7 @@
       </c>
     </row>
     <row r="5" spans="1:31" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="178" t="s">
+      <c r="A5" s="175" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -3406,7 +2853,7 @@
       </c>
     </row>
     <row r="6" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="179"/>
+      <c r="A6" s="176"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -3495,7 +2942,7 @@
       <c r="AE6" s="132"/>
     </row>
     <row r="7" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="179"/>
+      <c r="A7" s="176"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -3580,7 +3027,7 @@
       </c>
     </row>
     <row r="8" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="180"/>
+      <c r="A8" s="177"/>
       <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3668,7 +3115,7 @@
       </c>
     </row>
     <row r="9" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="181" t="s">
+      <c r="A9" s="178" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -3761,7 +3208,7 @@
       </c>
     </row>
     <row r="10" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="182"/>
+      <c r="A10" s="179"/>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -3849,7 +3296,7 @@
       <c r="AE10" s="47"/>
     </row>
     <row r="11" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="182"/>
+      <c r="A11" s="179"/>
       <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
@@ -3932,7 +3379,7 @@
       <c r="AE11" s="47"/>
     </row>
     <row r="12" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="183"/>
+      <c r="A12" s="180"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -4098,7 +3545,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE13" s="47"/>
+      <c r="AE13" s="155" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="14" spans="1:31" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
@@ -4133,14 +3582,14 @@
         <v>0</v>
       </c>
       <c r="S14" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="T14" s="160" t="s">
         <v>125</v>
-      </c>
-      <c r="T14" s="160" t="s">
-        <v>126</v>
       </c>
       <c r="U14" s="146"/>
       <c r="V14" s="159">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="W14" s="159">
         <v>0</v>
@@ -4149,7 +3598,7 @@
         <v>0</v>
       </c>
       <c r="Y14" s="159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z14" s="159">
         <v>0</v>
@@ -4206,38 +3655,38 @@
       </c>
       <c r="R15" s="132"/>
       <c r="S15" s="51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T15" s="160" t="s">
         <v>102</v>
       </c>
       <c r="U15" s="146"/>
       <c r="V15" s="58" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="W15" s="58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="X15" s="58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="Y15" s="58" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="Z15" s="58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AA15" s="58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AB15" s="58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AC15" s="58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AD15" s="58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4286,31 +3735,31 @@
       </c>
       <c r="U16" s="146"/>
       <c r="V16" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="W16" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="W16" s="58" t="s">
-        <v>124</v>
-      </c>
       <c r="X16" s="58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Y16" s="58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Z16" s="58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AA16" s="58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB16" s="58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AC16" s="58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AD16" s="58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:32" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4353,7 +3802,7 @@
       </c>
       <c r="R17" s="30"/>
       <c r="S17" s="51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="T17" s="49" t="s">
         <v>102</v>
@@ -4363,28 +3812,28 @@
         <v>121</v>
       </c>
       <c r="W17" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X17" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Y17" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z17" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AA17" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AB17" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AC17" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AD17" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:32" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4440,7 +3889,7 @@
         <v>113</v>
       </c>
       <c r="Y18" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z18" s="58" t="s">
         <v>113</v>
@@ -4510,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="Y19" s="145">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="Z19" s="145">
         <v>0</v>
@@ -4568,7 +4017,7 @@
         <v>1251.5450000000001</v>
       </c>
       <c r="S20" s="51" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="T20" s="49" t="s">
         <v>103</v>
@@ -4630,7 +4079,7 @@
       </c>
       <c r="U21" s="146"/>
       <c r="V21" s="58" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="W21" s="58" t="s">
         <v>113</v>
@@ -4677,14 +4126,14 @@
       <c r="P22" s="158"/>
       <c r="Q22" s="38"/>
       <c r="S22" s="51" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T22" s="160" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="U22" s="146"/>
       <c r="V22" s="159">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="W22" s="159">
         <v>0</v>
@@ -4693,7 +4142,7 @@
         <v>0</v>
       </c>
       <c r="Y22" s="159">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="Z22" s="159">
         <v>0</v>
@@ -4785,14 +4234,14 @@
       <c r="P24" s="157"/>
       <c r="Q24" s="38"/>
       <c r="S24" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T24" s="49" t="s">
         <v>98</v>
       </c>
       <c r="U24" s="146"/>
       <c r="V24" s="58" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="W24" s="58" t="s">
         <v>113</v>
@@ -4838,14 +4287,14 @@
       <c r="P25" s="157"/>
       <c r="Q25" s="38"/>
       <c r="S25" s="51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T25" s="49" t="s">
         <v>100</v>
       </c>
       <c r="U25" s="146"/>
       <c r="V25" s="58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W25" s="58">
         <v>0</v>
@@ -4874,14 +4323,14 @@
     </row>
     <row r="26" spans="1:32" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="S26" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T26" s="49" t="s">
         <v>100</v>
       </c>
       <c r="U26" s="146"/>
       <c r="V26" s="58">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W26" s="58">
         <v>0</v>
@@ -4914,19 +4363,6 @@
     <row r="30" spans="1:32" ht="46.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="P4:Q4"/>
@@ -4935,6 +4371,19 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
   </mergeCells>
   <conditionalFormatting sqref="B23">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
@@ -4971,8 +4420,7 @@
   <ignoredErrors>
     <ignoredError sqref="G16 E16 C16 V8" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5001,12 +4449,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="196" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="197"/>
-      <c r="C1" s="197"/>
-      <c r="D1" s="197"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
       <c r="E1" s="44"/>
       <c r="F1" s="14"/>
       <c r="G1" s="55"/>
@@ -5080,7 +4528,7 @@
       <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="198" t="s">
+      <c r="A4" s="197" t="s">
         <v>69</v>
       </c>
       <c r="B4" s="46"/>
@@ -5103,21 +4551,21 @@
       <c r="I4" s="62">
         <v>0.77584580000000003</v>
       </c>
-      <c r="J4" s="196" t="s">
+      <c r="J4" s="194" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="196" t="s">
+      <c r="K4" s="194" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="196" t="s">
+      <c r="L4" s="194" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="196" t="s">
+      <c r="M4" s="194" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="196"/>
+      <c r="A5" s="194"/>
       <c r="B5" s="46"/>
       <c r="C5" s="46"/>
       <c r="D5" s="12">
@@ -5138,13 +4586,13 @@
       <c r="I5" s="62">
         <v>1.45</v>
       </c>
-      <c r="J5" s="196"/>
-      <c r="K5" s="196"/>
-      <c r="L5" s="196"/>
-      <c r="M5" s="196"/>
+      <c r="J5" s="194"/>
+      <c r="K5" s="194"/>
+      <c r="L5" s="194"/>
+      <c r="M5" s="194"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="196"/>
+      <c r="A6" s="194"/>
       <c r="B6" s="46"/>
       <c r="C6" s="46"/>
       <c r="D6" s="12">
@@ -5165,13 +4613,13 @@
       <c r="I6" s="62">
         <v>10</v>
       </c>
-      <c r="J6" s="196"/>
-      <c r="K6" s="196"/>
-      <c r="L6" s="196"/>
-      <c r="M6" s="196"/>
+      <c r="J6" s="194"/>
+      <c r="K6" s="194"/>
+      <c r="L6" s="194"/>
+      <c r="M6" s="194"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="196"/>
+      <c r="A7" s="194"/>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
       <c r="D7" s="12">
@@ -5192,25 +4640,25 @@
       <c r="I7" s="62">
         <v>1</v>
       </c>
-      <c r="J7" s="196"/>
-      <c r="K7" s="196"/>
-      <c r="L7" s="196"/>
-      <c r="M7" s="196"/>
+      <c r="J7" s="194"/>
+      <c r="K7" s="194"/>
+      <c r="L7" s="194"/>
+      <c r="M7" s="194"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="196"/>
+      <c r="A8" s="194"/>
       <c r="B8" s="46"/>
       <c r="C8" s="46"/>
       <c r="D8" s="12">
         <v>4</v>
       </c>
-      <c r="J8" s="196"/>
-      <c r="K8" s="196"/>
-      <c r="L8" s="196"/>
-      <c r="M8" s="196"/>
+      <c r="J8" s="194"/>
+      <c r="K8" s="194"/>
+      <c r="L8" s="194"/>
+      <c r="M8" s="194"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="194"/>
+      <c r="A9" s="195"/>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="13">
@@ -5218,10 +4666,10 @@
       </c>
       <c r="H9" s="55"/>
       <c r="I9" s="55"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="194"/>
-      <c r="L9" s="194"/>
-      <c r="M9" s="194"/>
+      <c r="J9" s="195"/>
+      <c r="K9" s="195"/>
+      <c r="L9" s="195"/>
+      <c r="M9" s="195"/>
     </row>
     <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="192" t="s">
@@ -5253,11 +4701,11 @@
       <c r="M10" s="192" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="195" t="s">
+      <c r="N10" s="198" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="195"/>
-      <c r="P10" s="195"/>
+      <c r="O10" s="198"/>
+      <c r="P10" s="198"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="193"/>
@@ -5279,9 +4727,9 @@
       <c r="K11" s="193"/>
       <c r="L11" s="193"/>
       <c r="M11" s="193"/>
-      <c r="N11" s="195"/>
-      <c r="O11" s="195"/>
-      <c r="P11" s="195"/>
+      <c r="N11" s="198"/>
+      <c r="O11" s="198"/>
+      <c r="P11" s="198"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="193"/>
@@ -5297,13 +4745,13 @@
         <v>30</v>
       </c>
       <c r="I12" s="12"/>
-      <c r="J12" s="196"/>
-      <c r="K12" s="196"/>
-      <c r="L12" s="196"/>
-      <c r="M12" s="196"/>
-      <c r="N12" s="195"/>
-      <c r="O12" s="195"/>
-      <c r="P12" s="195"/>
+      <c r="J12" s="194"/>
+      <c r="K12" s="194"/>
+      <c r="L12" s="194"/>
+      <c r="M12" s="194"/>
+      <c r="N12" s="198"/>
+      <c r="O12" s="198"/>
+      <c r="P12" s="198"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="193"/>
@@ -5317,13 +4765,13 @@
       <c r="G13" s="53"/>
       <c r="H13" s="53"/>
       <c r="I13" s="12"/>
-      <c r="J13" s="196"/>
-      <c r="K13" s="196"/>
-      <c r="L13" s="196"/>
-      <c r="M13" s="196"/>
-      <c r="N13" s="195"/>
-      <c r="O13" s="195"/>
-      <c r="P13" s="195"/>
+      <c r="J13" s="194"/>
+      <c r="K13" s="194"/>
+      <c r="L13" s="194"/>
+      <c r="M13" s="194"/>
+      <c r="N13" s="198"/>
+      <c r="O13" s="198"/>
+      <c r="P13" s="198"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="193"/>
@@ -5337,16 +4785,16 @@
       <c r="G14" s="53"/>
       <c r="H14" s="53"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="196"/>
-      <c r="K14" s="196"/>
-      <c r="L14" s="196"/>
-      <c r="M14" s="196"/>
-      <c r="N14" s="195"/>
-      <c r="O14" s="195"/>
-      <c r="P14" s="195"/>
+      <c r="J14" s="194"/>
+      <c r="K14" s="194"/>
+      <c r="L14" s="194"/>
+      <c r="M14" s="194"/>
+      <c r="N14" s="198"/>
+      <c r="O14" s="198"/>
+      <c r="P14" s="198"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="194"/>
+      <c r="A15" s="195"/>
       <c r="B15" s="44"/>
       <c r="C15" s="55"/>
       <c r="D15" s="13">
@@ -5357,13 +4805,13 @@
       <c r="G15" s="53"/>
       <c r="H15" s="55"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="194"/>
-      <c r="K15" s="194"/>
-      <c r="L15" s="194"/>
-      <c r="M15" s="194"/>
-      <c r="N15" s="195"/>
-      <c r="O15" s="195"/>
-      <c r="P15" s="195"/>
+      <c r="J15" s="195"/>
+      <c r="K15" s="195"/>
+      <c r="L15" s="195"/>
+      <c r="M15" s="195"/>
+      <c r="N15" s="198"/>
+      <c r="O15" s="198"/>
+      <c r="P15" s="198"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="192" t="s">
@@ -5532,10 +4980,10 @@
       <c r="I21" s="55">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J21" s="196"/>
-      <c r="K21" s="196"/>
-      <c r="L21" s="196"/>
-      <c r="M21" s="196"/>
+      <c r="J21" s="194"/>
+      <c r="K21" s="194"/>
+      <c r="L21" s="194"/>
+      <c r="M21" s="194"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="192" t="s">
@@ -5683,7 +5131,7 @@
       <c r="M26" s="193"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="194"/>
+      <c r="A27" s="195"/>
       <c r="B27" s="44"/>
       <c r="C27" s="55"/>
       <c r="D27" s="13">
@@ -5704,10 +5152,10 @@
       <c r="I27" s="55">
         <v>1.38</v>
       </c>
-      <c r="J27" s="194"/>
-      <c r="K27" s="194"/>
-      <c r="L27" s="194"/>
-      <c r="M27" s="194"/>
+      <c r="J27" s="195"/>
+      <c r="K27" s="195"/>
+      <c r="L27" s="195"/>
+      <c r="M27" s="195"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="192" t="s">
@@ -5797,7 +5245,7 @@
       <c r="M32" s="193"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="194"/>
+      <c r="A33" s="195"/>
       <c r="B33" s="79"/>
       <c r="C33" s="79"/>
       <c r="D33" s="13">
@@ -5808,10 +5256,10 @@
       <c r="G33" s="79"/>
       <c r="H33" s="79"/>
       <c r="I33" s="79"/>
-      <c r="J33" s="194"/>
-      <c r="K33" s="194"/>
-      <c r="L33" s="194"/>
-      <c r="M33" s="194"/>
+      <c r="J33" s="195"/>
+      <c r="K33" s="195"/>
+      <c r="L33" s="195"/>
+      <c r="M33" s="195"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="192" t="s">
@@ -5901,7 +5349,7 @@
       <c r="M38" s="193"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="194"/>
+      <c r="A39" s="195"/>
       <c r="B39" s="79"/>
       <c r="C39" s="79"/>
       <c r="D39" s="13">
@@ -5912,10 +5360,10 @@
       <c r="G39" s="79"/>
       <c r="H39" s="79"/>
       <c r="I39" s="79"/>
-      <c r="J39" s="194"/>
-      <c r="K39" s="194"/>
-      <c r="L39" s="194"/>
-      <c r="M39" s="194"/>
+      <c r="J39" s="195"/>
+      <c r="K39" s="195"/>
+      <c r="L39" s="195"/>
+      <c r="M39" s="195"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="52" t="s">
@@ -6062,7 +5510,7 @@
       <c r="M46" s="193"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" s="194"/>
+      <c r="A47" s="195"/>
       <c r="B47" s="152"/>
       <c r="C47" s="152"/>
       <c r="D47" s="13">
@@ -6073,26 +5521,28 @@
       <c r="G47" s="152"/>
       <c r="H47" s="152"/>
       <c r="I47" s="152"/>
-      <c r="J47" s="194"/>
-      <c r="K47" s="194"/>
-      <c r="L47" s="194"/>
-      <c r="M47" s="194"/>
+      <c r="J47" s="195"/>
+      <c r="K47" s="195"/>
+      <c r="L47" s="195"/>
+      <c r="M47" s="195"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="L16:L21"/>
-    <mergeCell ref="M16:M21"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="J22:J27"/>
-    <mergeCell ref="K22:K27"/>
-    <mergeCell ref="L22:L27"/>
-    <mergeCell ref="M22:M27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="K16:K21"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="J16:J21"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="J42:J47"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="M42:M47"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="J34:J39"/>
+    <mergeCell ref="K34:K39"/>
+    <mergeCell ref="L34:L39"/>
+    <mergeCell ref="M34:M39"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="J28:J33"/>
+    <mergeCell ref="K28:K33"/>
+    <mergeCell ref="L28:L33"/>
+    <mergeCell ref="M28:M33"/>
     <mergeCell ref="N10:P15"/>
     <mergeCell ref="M10:M15"/>
     <mergeCell ref="J4:J9"/>
@@ -6102,21 +5552,19 @@
     <mergeCell ref="J10:J15"/>
     <mergeCell ref="K10:K15"/>
     <mergeCell ref="L10:L15"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="J28:J33"/>
-    <mergeCell ref="K28:K33"/>
-    <mergeCell ref="L28:L33"/>
-    <mergeCell ref="M28:M33"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="J34:J39"/>
-    <mergeCell ref="K34:K39"/>
-    <mergeCell ref="L34:L39"/>
-    <mergeCell ref="M34:M39"/>
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="J42:J47"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="M42:M47"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="K16:K21"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="J16:J21"/>
+    <mergeCell ref="L16:L21"/>
+    <mergeCell ref="M16:M21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="J22:J27"/>
+    <mergeCell ref="K22:K27"/>
+    <mergeCell ref="L22:L27"/>
+    <mergeCell ref="M22:M27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Update of input mask for swimming pools
</commit_message>
<xml_diff>
--- a/teaser/examples/2021-03-24_Hüllflächen_Zonen_Shells_of_Zones.xlsx
+++ b/teaser/examples/2021-03-24_Hüllflächen_Zonen_Shells_of_Zones.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr codeName="DieseArbeitsmappe"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\TEASER\teaser\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EESchwimm\TEASER\teaser\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70A6A2B-90C6-40DE-98B3-CA9F9E7014E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hüllflächen, Himmelsricht." sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <definedName name="GlassA" localSheetId="1">[1]Dropdown!#REF!</definedName>
     <definedName name="GlassA">[1]Dropdown!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={7F796FA0-45EC-4C4C-843B-360D0385E38E}</author>
     <author>tc={F73AF337-B134-4C39-9107-82E90BF9956F}</author>
@@ -58,87 +57,177 @@
     <author>tc={E2D2AD93-2ABA-461B-840E-EE396FE1B71C}</author>
   </authors>
   <commentList>
-    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{7F796FA0-45EC-4C4C-843B-360D0385E38E}">
+    <comment ref="J4" authorId="0" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     Zone in Zone?
 Vorschlag: Wände zur Schwimmhalle als innere Wände addieren um Wärmekapazitäten zu berücksichtigen.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="V7" authorId="1" shapeId="0" xr:uid="{F73AF337-B134-4C39-9107-82E90BF9956F}">
+    <comment ref="V7" authorId="1" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     enthält Wand zum Technikraum * 0,5</t>
+        </r>
       </text>
     </comment>
-    <comment ref="V9" authorId="2" shapeId="0" xr:uid="{F4ECF03F-FA93-47D6-80B6-B15AA339D531}">
+    <comment ref="V9" authorId="2" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     enthält Wand zum Technikraum * 0,5</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G13" authorId="3" shapeId="0" xr:uid="{E25679EC-AF68-49A1-8507-B6CF62C08D43}">
+    <comment ref="G13" authorId="3" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     obere etage?</t>
+        </r>
       </text>
     </comment>
-    <comment ref="Q15" authorId="4" shapeId="0" xr:uid="{EC0811A3-7202-47EB-9217-80E3351DF89A}">
+    <comment ref="Q15" authorId="4" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     enthählt Wände zum Erdbooden</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="5" shapeId="0" xr:uid="{7F1FE8C0-BC0B-4180-A6B6-22AF3675656E}">
+    <comment ref="A16" authorId="5" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     Innere Wände ohne Kontakt mit anderen Zonen 
 + 
 (Innere Wände mit Kontakt mit anderen Zonen *0,5)</t>
+        </r>
       </text>
     </comment>
-    <comment ref="Q16" authorId="6" shapeId="0" xr:uid="{AFAD1E39-F4C4-4A33-952E-60446B18A8E1}">
+    <comment ref="Q16" authorId="6" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     enthählt wand zum schwimmbecken(*0,5)</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="7" shapeId="0" xr:uid="{243AE133-3DCA-48EA-A3CC-F3E7BB1287C4}">
+    <comment ref="A18" authorId="7" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     Abhangdecken?</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="8" shapeId="0" xr:uid="{BB49A417-0C91-4FBA-A209-8C9D51A02D76}">
+    <comment ref="G18" authorId="8" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     obere etage?</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="9" shapeId="0" xr:uid="{E2D2AD93-2ABA-461B-840E-EE396FE1B71C}">
+    <comment ref="I19" authorId="9" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     Ohne Wasserfläche</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -146,17 +235,26 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={B0FCD963-ED35-4353-B03A-99593B0E7AFB}</author>
   </authors>
   <commentList>
-    <comment ref="A41" authorId="0" shapeId="0" xr:uid="{B0FCD963-ED35-4353-B03A-99593B0E7AFB}">
+    <comment ref="A41" authorId="0" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     Horizontale Fenster werden in Teaser nicht erstellt</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -164,7 +262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="137">
   <si>
     <t>Zone 1</t>
   </si>
@@ -734,7 +832,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1583,7 +1681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2055,6 +2153,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2160,7 +2270,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 2" xfId="1"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -2539,72 +2649,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+      <selection activeCell="V5" sqref="V5:AD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="36" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="36" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="25"/>
-    <col min="6" max="6" width="13.33203125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="36" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="36" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="25"/>
+    <col min="6" max="6" width="13.28515625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="25" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="25"/>
-    <col min="10" max="10" width="11.44140625" style="25" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" style="25" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" style="25"/>
-    <col min="14" max="14" width="7.6640625" style="25" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" style="25"/>
-    <col min="16" max="16" width="7.6640625" style="25" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" style="25"/>
-    <col min="18" max="18" width="26.33203125" style="25" customWidth="1"/>
-    <col min="19" max="19" width="22.21875" style="25" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625" style="25" customWidth="1"/>
-    <col min="21" max="21" width="15.33203125" style="25" customWidth="1"/>
-    <col min="22" max="22" width="26.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.77734375" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.21875" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="25"/>
+    <col min="10" max="10" width="11.42578125" style="25" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="25" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="25"/>
+    <col min="14" max="14" width="7.7109375" style="25" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="25"/>
+    <col min="16" max="16" width="7.7109375" style="25" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="25"/>
+    <col min="18" max="18" width="26.28515625" style="25" customWidth="1"/>
+    <col min="19" max="19" width="22.28515625" style="25" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" style="25" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" style="25" customWidth="1"/>
+    <col min="22" max="22" width="26.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="29" style="25" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="18.44140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="11.44140625" style="25"/>
+    <col min="28" max="30" width="18.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="11.42578125" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1" s="187" t="s">
+    <row r="1" spans="1:31" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="191" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
-      <c r="I1" s="188"/>
-      <c r="J1" s="188"/>
-      <c r="K1" s="188"/>
-      <c r="L1" s="188"/>
-      <c r="M1" s="188"/>
-      <c r="N1" s="188"/>
-      <c r="O1" s="188"/>
-      <c r="P1" s="188"/>
-      <c r="Q1" s="188"/>
-    </row>
-    <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.3">
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
+      <c r="I1" s="192"/>
+      <c r="J1" s="192"/>
+      <c r="K1" s="192"/>
+      <c r="L1" s="192"/>
+      <c r="M1" s="192"/>
+      <c r="N1" s="192"/>
+      <c r="O1" s="192"/>
+      <c r="P1" s="192"/>
+      <c r="Q1" s="192"/>
+    </row>
+    <row r="2" spans="1:31" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="40"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -2623,44 +2733,44 @@
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
     </row>
-    <row r="3" spans="1:31" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="181" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="182"/>
-      <c r="D3" s="183" t="s">
+      <c r="B3" s="185" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="186"/>
+      <c r="D3" s="187" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="184"/>
-      <c r="F3" s="185" t="s">
+      <c r="E3" s="188"/>
+      <c r="F3" s="189" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="182"/>
-      <c r="H3" s="191" t="s">
+      <c r="G3" s="186"/>
+      <c r="H3" s="195" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="184"/>
-      <c r="J3" s="185" t="s">
+      <c r="I3" s="188"/>
+      <c r="J3" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="182"/>
-      <c r="L3" s="189" t="s">
+      <c r="K3" s="186"/>
+      <c r="L3" s="193" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="190"/>
-      <c r="N3" s="189" t="s">
+      <c r="M3" s="194"/>
+      <c r="N3" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="190"/>
-      <c r="P3" s="183" t="s">
+      <c r="O3" s="194"/>
+      <c r="P3" s="187" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="183"/>
-      <c r="S3" s="165" t="s">
+      <c r="Q3" s="187"/>
+      <c r="S3" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="T3" s="166"/>
+      <c r="T3" s="170"/>
       <c r="U3" s="163" t="s">
         <v>58</v>
       </c>
@@ -2692,44 +2802,44 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="186" t="s">
+      <c r="B4" s="190" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="169" t="s">
+      <c r="C4" s="174"/>
+      <c r="D4" s="173" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="170"/>
-      <c r="F4" s="169" t="s">
+      <c r="E4" s="174"/>
+      <c r="F4" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="170"/>
-      <c r="H4" s="169" t="s">
+      <c r="G4" s="174"/>
+      <c r="H4" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="170"/>
-      <c r="J4" s="171" t="s">
+      <c r="I4" s="174"/>
+      <c r="J4" s="175" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="172"/>
-      <c r="L4" s="173" t="s">
+      <c r="K4" s="176"/>
+      <c r="L4" s="177" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="174"/>
-      <c r="N4" s="173" t="s">
+      <c r="M4" s="178"/>
+      <c r="N4" s="177" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="174"/>
-      <c r="P4" s="169" t="s">
+      <c r="O4" s="178"/>
+      <c r="P4" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="186"/>
-      <c r="S4" s="167"/>
-      <c r="T4" s="168"/>
+      <c r="Q4" s="190"/>
+      <c r="S4" s="171"/>
+      <c r="T4" s="172"/>
       <c r="U4" s="48" t="s">
         <v>47</v>
       </c>
@@ -2761,8 +2871,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="175" t="s">
+    <row r="5" spans="1:31" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="179" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2820,7 +2930,7 @@
       </c>
       <c r="U5" s="146">
         <f t="shared" ref="U5:U10" si="0">SUM(V5:AD5)</f>
-        <v>541.5</v>
+        <v>552.79999999999995</v>
       </c>
       <c r="V5" s="144">
         <f>25*16.66</f>
@@ -2833,8 +2943,7 @@
         <v>0</v>
       </c>
       <c r="Y5" s="145">
-        <f>12.5*10</f>
-        <v>125</v>
+        <v>136.30000000000001</v>
       </c>
       <c r="Z5" s="57">
         <v>0</v>
@@ -2852,8 +2961,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="176"/>
+    <row r="6" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="180"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -2908,11 +3017,11 @@
       </c>
       <c r="U6" s="146">
         <f t="shared" si="0"/>
-        <v>716.32891940711272</v>
-      </c>
-      <c r="V6" s="145">
-        <f>V5+2.2*25*2+16.66*2</f>
-        <v>559.82000000000005</v>
+        <v>543.43000000000006</v>
+      </c>
+      <c r="V6" s="144">
+        <f>25*16.66</f>
+        <v>416.5</v>
       </c>
       <c r="W6" s="58">
         <v>0</v>
@@ -2921,8 +3030,7 @@
         <v>0</v>
       </c>
       <c r="Y6" s="145">
-        <f>1.35*12.5+SQRT(1.35^2+10^2)*12.5+1.35*10</f>
-        <v>156.5089194071127</v>
+        <v>126.93</v>
       </c>
       <c r="Z6" s="58">
         <v>0</v>
@@ -2941,8 +3049,8 @@
       </c>
       <c r="AE6" s="132"/>
     </row>
-    <row r="7" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="176"/>
+    <row r="7" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="180"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -3026,8 +3134,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="177"/>
+    <row r="8" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="181"/>
       <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3082,11 +3190,10 @@
       </c>
       <c r="U8" s="146">
         <f t="shared" si="0"/>
-        <v>299.82891940711272</v>
+        <v>183.666</v>
       </c>
       <c r="V8" s="145">
-        <f>V7+2.2*25*2+16.66*2</f>
-        <v>143.32000000000002</v>
+        <v>146.52000000000001</v>
       </c>
       <c r="W8" s="58">
         <v>0</v>
@@ -3095,8 +3202,7 @@
         <v>0</v>
       </c>
       <c r="Y8" s="145">
-        <f>1.35*12.5+SQRT(1.35^2+10^2)*12.5+1.35*10</f>
-        <v>156.5089194071127</v>
+        <v>37.146000000000001</v>
       </c>
       <c r="Z8" s="58">
         <v>0</v>
@@ -3114,8 +3220,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="178" t="s">
+    <row r="9" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="182" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -3173,11 +3279,10 @@
       </c>
       <c r="U9" s="146">
         <f t="shared" si="0"/>
-        <v>21.658000000000001</v>
+        <v>43.316000000000003</v>
       </c>
       <c r="V9" s="147">
-        <f>0.5*16.66*2.6</f>
-        <v>21.658000000000001</v>
+        <v>43.316000000000003</v>
       </c>
       <c r="W9" s="58">
         <v>0</v>
@@ -3207,8 +3312,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="179"/>
+    <row r="10" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="183"/>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -3262,11 +3367,10 @@
       </c>
       <c r="U10" s="146">
         <f t="shared" si="0"/>
-        <v>1000.6750000000001</v>
+        <v>1069.7560000000001</v>
       </c>
       <c r="V10" s="145">
-        <f>V5*2.2</f>
-        <v>916.30000000000007</v>
+        <v>942.95600000000002</v>
       </c>
       <c r="W10" s="58">
         <v>0</v>
@@ -3275,8 +3379,7 @@
         <v>0</v>
       </c>
       <c r="Y10" s="145">
-        <f>(10*12.5*1.35)/2</f>
-        <v>84.375</v>
+        <v>126.8</v>
       </c>
       <c r="Z10" s="58">
         <v>0</v>
@@ -3295,8 +3398,8 @@
       </c>
       <c r="AE10" s="47"/>
     </row>
-    <row r="11" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="179"/>
+    <row r="11" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="183"/>
       <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
@@ -3350,7 +3453,7 @@
       </c>
       <c r="U11" s="146"/>
       <c r="V11" s="58">
-        <v>303.14999999999998</v>
+        <v>301.14999999999998</v>
       </c>
       <c r="W11" s="58">
         <v>0</v>
@@ -3378,8 +3481,8 @@
       </c>
       <c r="AE11" s="47"/>
     </row>
-    <row r="12" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="180"/>
+    <row r="12" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="184"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -3464,7 +3567,7 @@
       </c>
       <c r="AE12" s="47"/>
     </row>
-    <row r="13" spans="1:31" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
         <v>42</v>
       </c>
@@ -3511,7 +3614,7 @@
       <c r="U13" s="146"/>
       <c r="V13" s="58">
         <f>IF(V5&gt;0,V10/V5,0)</f>
-        <v>2.2000000000000002</v>
+        <v>2.2640000000000002</v>
       </c>
       <c r="W13" s="58">
         <f t="shared" ref="W13:AD13" si="1">IF(W5&gt;0,W10/W5,0)</f>
@@ -3522,8 +3625,8 @@
         <v>0</v>
       </c>
       <c r="Y13" s="58">
-        <f t="shared" si="1"/>
-        <v>0.67500000000000004</v>
+        <f>IF(Y5&gt;0,Y10/Y5,0)</f>
+        <v>0.93030080704328677</v>
       </c>
       <c r="Z13" s="58">
         <f t="shared" si="1"/>
@@ -3549,7 +3652,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>17</v>
       </c>
@@ -3616,7 +3719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29" t="s">
         <v>90</v>
       </c>
@@ -3689,7 +3792,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="133" t="s">
         <v>89</v>
       </c>
@@ -3762,7 +3865,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:32" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29" t="s">
         <v>45</v>
       </c>
@@ -3836,7 +3939,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="133" t="s">
         <v>87</v>
       </c>
@@ -3907,7 +4010,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:32" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:32" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="37" t="s">
         <v>88</v>
       </c>
@@ -3978,7 +4081,7 @@
       </c>
       <c r="AF19" s="161"/>
     </row>
-    <row r="20" spans="1:32" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>18</v>
       </c>
@@ -4052,7 +4155,7 @@
       </c>
       <c r="AF20" s="161"/>
     </row>
-    <row r="21" spans="1:32" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" ht="58.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="156"/>
       <c r="B21" s="156"/>
       <c r="C21" s="38"/>
@@ -4107,7 +4210,7 @@
       </c>
       <c r="AF21" s="161"/>
     </row>
-    <row r="22" spans="1:32" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="158"/>
       <c r="B22" s="158"/>
       <c r="C22" s="158"/>
@@ -4161,7 +4264,7 @@
       </c>
       <c r="AF22" s="161"/>
     </row>
-    <row r="23" spans="1:32" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="157"/>
       <c r="C23" s="157"/>
@@ -4215,7 +4318,7 @@
       </c>
       <c r="AF23" s="161"/>
     </row>
-    <row r="24" spans="1:32" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
       <c r="B24" s="157"/>
       <c r="C24" s="157"/>
@@ -4268,7 +4371,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:32" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="157"/>
       <c r="C25" s="157"/>
@@ -4321,7 +4424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:32" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S26" s="51" t="s">
         <v>128</v>
       </c>
@@ -4357,10 +4460,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:32" ht="43.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:32" ht="46.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:32" ht="44.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:32" ht="46.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:32" ht="43.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:32" ht="46.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:32" ht="44.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:32" ht="46.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="A1:Q1"/>
@@ -4401,16 +4504,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V18:AD18 V21:AD21 V23:AD24" xr:uid="{45BA5B33-2983-4223-B859-793570591E1A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V18:AD18 V21:AD21 V23:AD24">
       <formula1>"True, False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V16:AD16" xr:uid="{6620303C-CAC9-4AAC-83D0-D6E818FFE2A0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V16:AD16">
       <formula1>"ohne Ozon, mit Ozon, mit Ultrafiltration, mit Brom"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V15:AD15" xr:uid="{B68B0368-0677-4929-8236-B6A66D68707F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V15:AD15">
       <formula1>"Aktivkohlefilter mit Ozon, geschlossener Schnellfilter, geschlossener Sorptionsfilter, offener Schnellfilter, offener Saugfilter, Quantozonfilter, Quarzkiesfilter, Zweischichtfilter, Zweischichtfilter mit Ozon"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V17:AD17" xr:uid="{B29952C6-BB82-4091-95D2-7433887FFB28}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V17:AD17">
       <formula1>"Salzwasser, Süßwasser"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4418,50 +4521,50 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="66" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G16 E16 C16 V8" formula="1"/>
+    <ignoredError sqref="G16 E16 C16" formula="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" style="8" customWidth="1"/>
-    <col min="2" max="3" width="16.88671875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="43" customWidth="1"/>
-    <col min="6" max="6" width="46.88671875" style="8" customWidth="1"/>
-    <col min="7" max="8" width="27.109375" style="54" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="8" customWidth="1"/>
+    <col min="2" max="3" width="16.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="43" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" style="8" customWidth="1"/>
+    <col min="7" max="8" width="27.140625" style="54" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="8" customWidth="1"/>
     <col min="10" max="10" width="0" style="8" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" style="8" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="8" hidden="1" customWidth="1"/>
     <col min="12" max="13" width="0" style="8" hidden="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="8"/>
+    <col min="14" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="196" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="200" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
       <c r="E1" s="44"/>
       <c r="F1" s="14"/>
       <c r="G1" s="55"/>
       <c r="H1" s="55"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:16" s="23" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="23" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>19</v>
       </c>
@@ -4502,7 +4605,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -4527,8 +4630,8 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="197" t="s">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="201" t="s">
         <v>69</v>
       </c>
       <c r="B4" s="46"/>
@@ -4551,28 +4654,43 @@
       <c r="I4" s="62">
         <v>0.77584580000000003</v>
       </c>
-      <c r="J4" s="194" t="s">
+      <c r="J4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="194" t="s">
+      <c r="K4" s="198" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="194" t="s">
+      <c r="L4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="194" t="s">
+      <c r="M4" s="198" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="194"/>
+      <c r="Q4" s="61">
+        <v>25</v>
+      </c>
+      <c r="R4" t="s">
+        <v>74</v>
+      </c>
+      <c r="S4" s="62">
+        <v>1.9375</v>
+      </c>
+      <c r="T4" s="62">
+        <v>2104.1999999999998</v>
+      </c>
+      <c r="U4" s="62">
+        <v>0.77584580000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="198"/>
       <c r="B5" s="46"/>
       <c r="C5" s="46"/>
       <c r="D5" s="12">
         <v>1</v>
       </c>
       <c r="E5" s="61">
-        <v>16</v>
+        <v>1600</v>
       </c>
       <c r="F5" t="s">
         <v>75</v>
@@ -4586,13 +4704,28 @@
       <c r="I5" s="62">
         <v>1.45</v>
       </c>
-      <c r="J5" s="194"/>
-      <c r="K5" s="194"/>
-      <c r="L5" s="194"/>
-      <c r="M5" s="194"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="194"/>
+      <c r="J5" s="198"/>
+      <c r="K5" s="198"/>
+      <c r="L5" s="198"/>
+      <c r="M5" s="198"/>
+      <c r="Q5" s="61">
+        <v>16</v>
+      </c>
+      <c r="R5" t="s">
+        <v>75</v>
+      </c>
+      <c r="S5" s="61">
+        <v>0.04</v>
+      </c>
+      <c r="T5" s="62">
+        <v>31</v>
+      </c>
+      <c r="U5" s="62">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="198"/>
       <c r="B6" s="46"/>
       <c r="C6" s="46"/>
       <c r="D6" s="12">
@@ -4613,13 +4746,28 @@
       <c r="I6" s="62">
         <v>10</v>
       </c>
-      <c r="J6" s="194"/>
-      <c r="K6" s="194"/>
-      <c r="L6" s="194"/>
-      <c r="M6" s="194"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="194"/>
+      <c r="J6" s="198"/>
+      <c r="K6" s="198"/>
+      <c r="L6" s="198"/>
+      <c r="M6" s="198"/>
+      <c r="Q6" s="61">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="s">
+        <v>76</v>
+      </c>
+      <c r="S6" s="62">
+        <v>0.7</v>
+      </c>
+      <c r="T6" s="62">
+        <v>1645</v>
+      </c>
+      <c r="U6" s="62">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="198"/>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
       <c r="D7" s="12">
@@ -4640,25 +4788,40 @@
       <c r="I7" s="62">
         <v>1</v>
       </c>
-      <c r="J7" s="194"/>
-      <c r="K7" s="194"/>
-      <c r="L7" s="194"/>
-      <c r="M7" s="194"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="194"/>
+      <c r="J7" s="198"/>
+      <c r="K7" s="198"/>
+      <c r="L7" s="198"/>
+      <c r="M7" s="198"/>
+      <c r="Q7" s="61">
+        <v>0.3</v>
+      </c>
+      <c r="R7" t="s">
+        <v>77</v>
+      </c>
+      <c r="S7" s="61">
+        <v>0.7</v>
+      </c>
+      <c r="T7" s="62">
+        <v>1690</v>
+      </c>
+      <c r="U7" s="62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="198"/>
       <c r="B8" s="46"/>
       <c r="C8" s="46"/>
       <c r="D8" s="12">
         <v>4</v>
       </c>
-      <c r="J8" s="194"/>
-      <c r="K8" s="194"/>
-      <c r="L8" s="194"/>
-      <c r="M8" s="194"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="195"/>
+      <c r="J8" s="198"/>
+      <c r="K8" s="198"/>
+      <c r="L8" s="198"/>
+      <c r="M8" s="198"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="199"/>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="13">
@@ -4666,13 +4829,13 @@
       </c>
       <c r="H9" s="55"/>
       <c r="I9" s="55"/>
-      <c r="J9" s="195"/>
-      <c r="K9" s="195"/>
-      <c r="L9" s="195"/>
-      <c r="M9" s="195"/>
-    </row>
-    <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="192" t="s">
+      <c r="J9" s="199"/>
+      <c r="K9" s="199"/>
+      <c r="L9" s="199"/>
+      <c r="M9" s="199"/>
+    </row>
+    <row r="10" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="196" t="s">
         <v>70</v>
       </c>
       <c r="B10" s="41"/>
@@ -4689,26 +4852,26 @@
       <c r="G10" s="52"/>
       <c r="H10" s="52"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="192" t="s">
+      <c r="J10" s="196" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="192" t="s">
+      <c r="K10" s="196" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="192" t="s">
+      <c r="L10" s="196" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="192" t="s">
+      <c r="M10" s="196" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="198" t="s">
+      <c r="N10" s="202" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="198"/>
-      <c r="P10" s="198"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="193"/>
+      <c r="O10" s="202"/>
+      <c r="P10" s="202"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="197"/>
       <c r="B11" s="42"/>
       <c r="C11" s="53"/>
       <c r="D11" s="18">
@@ -4723,16 +4886,16 @@
       <c r="G11" s="53"/>
       <c r="H11" s="53"/>
       <c r="I11" s="12"/>
-      <c r="J11" s="193"/>
-      <c r="K11" s="193"/>
-      <c r="L11" s="193"/>
-      <c r="M11" s="193"/>
-      <c r="N11" s="198"/>
-      <c r="O11" s="198"/>
-      <c r="P11" s="198"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="193"/>
+      <c r="J11" s="197"/>
+      <c r="K11" s="197"/>
+      <c r="L11" s="197"/>
+      <c r="M11" s="197"/>
+      <c r="N11" s="202"/>
+      <c r="O11" s="202"/>
+      <c r="P11" s="202"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="197"/>
       <c r="B12" s="42"/>
       <c r="C12" s="53"/>
       <c r="D12" s="12">
@@ -4745,16 +4908,16 @@
         <v>30</v>
       </c>
       <c r="I12" s="12"/>
-      <c r="J12" s="194"/>
-      <c r="K12" s="194"/>
-      <c r="L12" s="194"/>
-      <c r="M12" s="194"/>
-      <c r="N12" s="198"/>
-      <c r="O12" s="198"/>
-      <c r="P12" s="198"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="193"/>
+      <c r="J12" s="198"/>
+      <c r="K12" s="198"/>
+      <c r="L12" s="198"/>
+      <c r="M12" s="198"/>
+      <c r="N12" s="202"/>
+      <c r="O12" s="202"/>
+      <c r="P12" s="202"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="197"/>
       <c r="B13" s="42"/>
       <c r="C13" s="53"/>
       <c r="D13" s="12">
@@ -4765,16 +4928,16 @@
       <c r="G13" s="53"/>
       <c r="H13" s="53"/>
       <c r="I13" s="12"/>
-      <c r="J13" s="194"/>
-      <c r="K13" s="194"/>
-      <c r="L13" s="194"/>
-      <c r="M13" s="194"/>
-      <c r="N13" s="198"/>
-      <c r="O13" s="198"/>
-      <c r="P13" s="198"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="193"/>
+      <c r="J13" s="198"/>
+      <c r="K13" s="198"/>
+      <c r="L13" s="198"/>
+      <c r="M13" s="198"/>
+      <c r="N13" s="202"/>
+      <c r="O13" s="202"/>
+      <c r="P13" s="202"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="197"/>
       <c r="B14" s="53"/>
       <c r="C14" s="53"/>
       <c r="D14" s="12">
@@ -4785,16 +4948,16 @@
       <c r="G14" s="53"/>
       <c r="H14" s="53"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="194"/>
-      <c r="K14" s="194"/>
-      <c r="L14" s="194"/>
-      <c r="M14" s="194"/>
-      <c r="N14" s="198"/>
-      <c r="O14" s="198"/>
-      <c r="P14" s="198"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="195"/>
+      <c r="J14" s="198"/>
+      <c r="K14" s="198"/>
+      <c r="L14" s="198"/>
+      <c r="M14" s="198"/>
+      <c r="N14" s="202"/>
+      <c r="O14" s="202"/>
+      <c r="P14" s="202"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="199"/>
       <c r="B15" s="44"/>
       <c r="C15" s="55"/>
       <c r="D15" s="13">
@@ -4805,16 +4968,16 @@
       <c r="G15" s="53"/>
       <c r="H15" s="55"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="195"/>
-      <c r="K15" s="195"/>
-      <c r="L15" s="195"/>
-      <c r="M15" s="195"/>
-      <c r="N15" s="198"/>
-      <c r="O15" s="198"/>
-      <c r="P15" s="198"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="192" t="s">
+      <c r="J15" s="199"/>
+      <c r="K15" s="199"/>
+      <c r="L15" s="199"/>
+      <c r="M15" s="199"/>
+      <c r="N15" s="202"/>
+      <c r="O15" s="202"/>
+      <c r="P15" s="202"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="196" t="s">
         <v>86</v>
       </c>
       <c r="B16" s="16"/>
@@ -4837,21 +5000,21 @@
       <c r="I16" s="52">
         <v>0.47699999999999998</v>
       </c>
-      <c r="J16" s="192" t="s">
+      <c r="J16" s="196" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="192" t="s">
+      <c r="K16" s="196" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="192" t="s">
+      <c r="L16" s="196" t="s">
         <v>27</v>
       </c>
-      <c r="M16" s="192" t="s">
+      <c r="M16" s="196" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="193"/>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="197"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="18">
@@ -4872,13 +5035,13 @@
       <c r="I17" s="53">
         <v>1</v>
       </c>
-      <c r="J17" s="193"/>
-      <c r="K17" s="193"/>
-      <c r="L17" s="193"/>
-      <c r="M17" s="193"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="193"/>
+      <c r="J17" s="197"/>
+      <c r="K17" s="197"/>
+      <c r="L17" s="197"/>
+      <c r="M17" s="197"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="197"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="18">
@@ -4899,13 +5062,13 @@
       <c r="I18" s="53">
         <v>1.45</v>
       </c>
-      <c r="J18" s="193"/>
-      <c r="K18" s="193"/>
-      <c r="L18" s="193"/>
-      <c r="M18" s="193"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="193"/>
+      <c r="J18" s="197"/>
+      <c r="K18" s="197"/>
+      <c r="L18" s="197"/>
+      <c r="M18" s="197"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="197"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="18">
@@ -4926,13 +5089,13 @@
       <c r="I19" s="53">
         <v>1.45</v>
       </c>
-      <c r="J19" s="193"/>
-      <c r="K19" s="193"/>
-      <c r="L19" s="193"/>
-      <c r="M19" s="193"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="193"/>
+      <c r="J19" s="197"/>
+      <c r="K19" s="197"/>
+      <c r="L19" s="197"/>
+      <c r="M19" s="197"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="197"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="18">
@@ -4953,13 +5116,13 @@
       <c r="I20" s="53">
         <v>1</v>
       </c>
-      <c r="J20" s="193"/>
-      <c r="K20" s="193"/>
-      <c r="L20" s="193"/>
-      <c r="M20" s="193"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="193"/>
+      <c r="J20" s="197"/>
+      <c r="K20" s="197"/>
+      <c r="L20" s="197"/>
+      <c r="M20" s="197"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="197"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="18">
@@ -4980,13 +5143,13 @@
       <c r="I21" s="55">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J21" s="194"/>
-      <c r="K21" s="194"/>
-      <c r="L21" s="194"/>
-      <c r="M21" s="194"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="192" t="s">
+      <c r="J21" s="198"/>
+      <c r="K21" s="198"/>
+      <c r="L21" s="198"/>
+      <c r="M21" s="198"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="196" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="41"/>
@@ -5009,21 +5172,36 @@
       <c r="I22" s="65">
         <v>2</v>
       </c>
-      <c r="J22" s="192" t="s">
+      <c r="J22" s="196" t="s">
         <v>27</v>
       </c>
-      <c r="K22" s="192" t="s">
+      <c r="K22" s="196" t="s">
         <v>28</v>
       </c>
-      <c r="L22" s="192" t="s">
+      <c r="L22" s="196" t="s">
         <v>27</v>
       </c>
-      <c r="M22" s="192" t="s">
+      <c r="M22" s="196" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="193"/>
+      <c r="Q22" s="165">
+        <v>5</v>
+      </c>
+      <c r="R22" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="S22" s="165">
+        <v>1.4</v>
+      </c>
+      <c r="T22" s="165">
+        <v>250</v>
+      </c>
+      <c r="U22" s="65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="197"/>
       <c r="B23" s="42"/>
       <c r="C23" s="53"/>
       <c r="D23" s="18">
@@ -5044,13 +5222,28 @@
       <c r="I23" s="65">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J23" s="193"/>
-      <c r="K23" s="193"/>
-      <c r="L23" s="193"/>
-      <c r="M23" s="193"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="193"/>
+      <c r="J23" s="197"/>
+      <c r="K23" s="197"/>
+      <c r="L23" s="197"/>
+      <c r="M23" s="197"/>
+      <c r="Q23" s="166">
+        <v>0.2</v>
+      </c>
+      <c r="R23" t="s">
+        <v>34</v>
+      </c>
+      <c r="S23" s="166">
+        <v>0.35</v>
+      </c>
+      <c r="T23" s="166">
+        <v>900</v>
+      </c>
+      <c r="U23" s="65">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="197"/>
       <c r="B24" s="53"/>
       <c r="C24" s="53"/>
       <c r="D24" s="18">
@@ -5071,13 +5264,28 @@
       <c r="I24" s="65">
         <v>2</v>
       </c>
-      <c r="J24" s="193"/>
-      <c r="K24" s="193"/>
-      <c r="L24" s="193"/>
-      <c r="M24" s="193"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="193"/>
+      <c r="J24" s="197"/>
+      <c r="K24" s="197"/>
+      <c r="L24" s="197"/>
+      <c r="M24" s="197"/>
+      <c r="Q24" s="166">
+        <v>5</v>
+      </c>
+      <c r="R24" t="s">
+        <v>32</v>
+      </c>
+      <c r="S24" s="166">
+        <v>1.4</v>
+      </c>
+      <c r="T24" s="166">
+        <v>250</v>
+      </c>
+      <c r="U24" s="65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="197"/>
       <c r="B25" s="53"/>
       <c r="C25" s="53"/>
       <c r="D25" s="18">
@@ -5098,13 +5306,28 @@
       <c r="I25" s="65">
         <v>0.77584580000000003</v>
       </c>
-      <c r="J25" s="193"/>
-      <c r="K25" s="193"/>
-      <c r="L25" s="193"/>
-      <c r="M25" s="193"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="193"/>
+      <c r="J25" s="197"/>
+      <c r="K25" s="197"/>
+      <c r="L25" s="197"/>
+      <c r="M25" s="197"/>
+      <c r="Q25" s="166">
+        <v>20</v>
+      </c>
+      <c r="R25" t="s">
+        <v>74</v>
+      </c>
+      <c r="S25" s="166">
+        <v>1.94</v>
+      </c>
+      <c r="T25" s="166">
+        <v>2104.1999999999998</v>
+      </c>
+      <c r="U25" s="65">
+        <v>0.77584580000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="197"/>
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
       <c r="D26" s="18">
@@ -5125,13 +5348,28 @@
       <c r="I26" s="54">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J26" s="193"/>
-      <c r="K26" s="193"/>
-      <c r="L26" s="193"/>
-      <c r="M26" s="193"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="195"/>
+      <c r="J26" s="197"/>
+      <c r="K26" s="197"/>
+      <c r="L26" s="197"/>
+      <c r="M26" s="197"/>
+      <c r="Q26" s="166">
+        <v>0.2</v>
+      </c>
+      <c r="R26" t="s">
+        <v>34</v>
+      </c>
+      <c r="S26" s="166">
+        <v>0.35</v>
+      </c>
+      <c r="T26" s="166">
+        <v>900</v>
+      </c>
+      <c r="U26" s="167">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="199"/>
       <c r="B27" s="44"/>
       <c r="C27" s="55"/>
       <c r="D27" s="13">
@@ -5152,13 +5390,28 @@
       <c r="I27" s="55">
         <v>1.38</v>
       </c>
-      <c r="J27" s="195"/>
-      <c r="K27" s="195"/>
-      <c r="L27" s="195"/>
-      <c r="M27" s="195"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="192" t="s">
+      <c r="J27" s="199"/>
+      <c r="K27" s="199"/>
+      <c r="L27" s="199"/>
+      <c r="M27" s="199"/>
+      <c r="Q27" s="168">
+        <v>10</v>
+      </c>
+      <c r="R27" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="S27" s="168">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="T27" s="168">
+        <v>30</v>
+      </c>
+      <c r="U27" s="168">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="196" t="s">
         <v>96</v>
       </c>
       <c r="B28" s="76"/>
@@ -5171,13 +5424,13 @@
       <c r="G28" s="76"/>
       <c r="H28" s="76"/>
       <c r="I28" s="65"/>
-      <c r="J28" s="192"/>
-      <c r="K28" s="192"/>
-      <c r="L28" s="192"/>
-      <c r="M28" s="192"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="193"/>
+      <c r="J28" s="196"/>
+      <c r="K28" s="196"/>
+      <c r="L28" s="196"/>
+      <c r="M28" s="196"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="197"/>
       <c r="B29" s="77"/>
       <c r="C29" s="77"/>
       <c r="D29" s="18">
@@ -5188,13 +5441,13 @@
       <c r="G29" s="77"/>
       <c r="H29" s="77"/>
       <c r="I29" s="65"/>
-      <c r="J29" s="193"/>
-      <c r="K29" s="193"/>
-      <c r="L29" s="193"/>
-      <c r="M29" s="193"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="193"/>
+      <c r="J29" s="197"/>
+      <c r="K29" s="197"/>
+      <c r="L29" s="197"/>
+      <c r="M29" s="197"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="197"/>
       <c r="B30" s="77"/>
       <c r="C30" s="77"/>
       <c r="D30" s="18">
@@ -5205,13 +5458,13 @@
       <c r="G30" s="77"/>
       <c r="H30" s="77"/>
       <c r="I30" s="65"/>
-      <c r="J30" s="193"/>
-      <c r="K30" s="193"/>
-      <c r="L30" s="193"/>
-      <c r="M30" s="193"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="193"/>
+      <c r="J30" s="197"/>
+      <c r="K30" s="197"/>
+      <c r="L30" s="197"/>
+      <c r="M30" s="197"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="197"/>
       <c r="B31" s="77"/>
       <c r="C31" s="77"/>
       <c r="D31" s="18">
@@ -5222,13 +5475,13 @@
       <c r="G31" s="77"/>
       <c r="H31" s="77"/>
       <c r="I31" s="65"/>
-      <c r="J31" s="193"/>
-      <c r="K31" s="193"/>
-      <c r="L31" s="193"/>
-      <c r="M31" s="193"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="193"/>
+      <c r="J31" s="197"/>
+      <c r="K31" s="197"/>
+      <c r="L31" s="197"/>
+      <c r="M31" s="197"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="197"/>
       <c r="B32" s="77"/>
       <c r="C32" s="77"/>
       <c r="D32" s="18">
@@ -5239,13 +5492,13 @@
       <c r="G32" s="77"/>
       <c r="H32" s="77"/>
       <c r="I32" s="78"/>
-      <c r="J32" s="193"/>
-      <c r="K32" s="193"/>
-      <c r="L32" s="193"/>
-      <c r="M32" s="193"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="195"/>
+      <c r="J32" s="197"/>
+      <c r="K32" s="197"/>
+      <c r="L32" s="197"/>
+      <c r="M32" s="197"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="199"/>
       <c r="B33" s="79"/>
       <c r="C33" s="79"/>
       <c r="D33" s="13">
@@ -5256,13 +5509,13 @@
       <c r="G33" s="79"/>
       <c r="H33" s="79"/>
       <c r="I33" s="79"/>
-      <c r="J33" s="195"/>
-      <c r="K33" s="195"/>
-      <c r="L33" s="195"/>
-      <c r="M33" s="195"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="192" t="s">
+      <c r="J33" s="199"/>
+      <c r="K33" s="199"/>
+      <c r="L33" s="199"/>
+      <c r="M33" s="199"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="196" t="s">
         <v>95</v>
       </c>
       <c r="B34" s="76"/>
@@ -5275,13 +5528,13 @@
       <c r="G34" s="76"/>
       <c r="H34" s="76"/>
       <c r="I34" s="65"/>
-      <c r="J34" s="192"/>
-      <c r="K34" s="192"/>
-      <c r="L34" s="192"/>
-      <c r="M34" s="192"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="193"/>
+      <c r="J34" s="196"/>
+      <c r="K34" s="196"/>
+      <c r="L34" s="196"/>
+      <c r="M34" s="196"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="197"/>
       <c r="B35" s="77"/>
       <c r="C35" s="77"/>
       <c r="D35" s="18">
@@ -5292,13 +5545,13 @@
       <c r="G35" s="77"/>
       <c r="H35" s="77"/>
       <c r="I35" s="65"/>
-      <c r="J35" s="193"/>
-      <c r="K35" s="193"/>
-      <c r="L35" s="193"/>
-      <c r="M35" s="193"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="193"/>
+      <c r="J35" s="197"/>
+      <c r="K35" s="197"/>
+      <c r="L35" s="197"/>
+      <c r="M35" s="197"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="197"/>
       <c r="B36" s="77"/>
       <c r="C36" s="77"/>
       <c r="D36" s="18">
@@ -5309,13 +5562,13 @@
       <c r="G36" s="77"/>
       <c r="H36" s="77"/>
       <c r="I36" s="65"/>
-      <c r="J36" s="193"/>
-      <c r="K36" s="193"/>
-      <c r="L36" s="193"/>
-      <c r="M36" s="193"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" s="193"/>
+      <c r="J36" s="197"/>
+      <c r="K36" s="197"/>
+      <c r="L36" s="197"/>
+      <c r="M36" s="197"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="197"/>
       <c r="B37" s="77"/>
       <c r="C37" s="77"/>
       <c r="D37" s="18">
@@ -5326,13 +5579,13 @@
       <c r="G37" s="77"/>
       <c r="H37" s="77"/>
       <c r="I37" s="65"/>
-      <c r="J37" s="193"/>
-      <c r="K37" s="193"/>
-      <c r="L37" s="193"/>
-      <c r="M37" s="193"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="193"/>
+      <c r="J37" s="197"/>
+      <c r="K37" s="197"/>
+      <c r="L37" s="197"/>
+      <c r="M37" s="197"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="197"/>
       <c r="B38" s="77"/>
       <c r="C38" s="77"/>
       <c r="D38" s="18">
@@ -5343,13 +5596,13 @@
       <c r="G38" s="77"/>
       <c r="H38" s="77"/>
       <c r="I38" s="78"/>
-      <c r="J38" s="193"/>
-      <c r="K38" s="193"/>
-      <c r="L38" s="193"/>
-      <c r="M38" s="193"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="195"/>
+      <c r="J38" s="197"/>
+      <c r="K38" s="197"/>
+      <c r="L38" s="197"/>
+      <c r="M38" s="197"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="199"/>
       <c r="B39" s="79"/>
       <c r="C39" s="79"/>
       <c r="D39" s="13">
@@ -5360,12 +5613,12 @@
       <c r="G39" s="79"/>
       <c r="H39" s="79"/>
       <c r="I39" s="79"/>
-      <c r="J39" s="195"/>
-      <c r="K39" s="195"/>
-      <c r="L39" s="195"/>
-      <c r="M39" s="195"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J39" s="199"/>
+      <c r="K39" s="199"/>
+      <c r="L39" s="199"/>
+      <c r="M39" s="199"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="52" t="s">
         <v>109</v>
       </c>
@@ -5406,7 +5659,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="154" t="s">
         <v>72</v>
       </c>
@@ -5422,8 +5675,8 @@
       <c r="L41" s="71"/>
       <c r="M41" s="71"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A42" s="192" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="196" t="s">
         <v>104</v>
       </c>
       <c r="B42" s="150"/>
@@ -5436,13 +5689,13 @@
       <c r="G42" s="150"/>
       <c r="H42" s="150"/>
       <c r="I42" s="65"/>
-      <c r="J42" s="192"/>
-      <c r="K42" s="192"/>
-      <c r="L42" s="192"/>
-      <c r="M42" s="192"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A43" s="193"/>
+      <c r="J42" s="196"/>
+      <c r="K42" s="196"/>
+      <c r="L42" s="196"/>
+      <c r="M42" s="196"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="197"/>
       <c r="B43" s="151"/>
       <c r="C43" s="151"/>
       <c r="D43" s="18">
@@ -5453,13 +5706,13 @@
       <c r="G43" s="151"/>
       <c r="H43" s="151"/>
       <c r="I43" s="65"/>
-      <c r="J43" s="193"/>
-      <c r="K43" s="193"/>
-      <c r="L43" s="193"/>
-      <c r="M43" s="193"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A44" s="193"/>
+      <c r="J43" s="197"/>
+      <c r="K43" s="197"/>
+      <c r="L43" s="197"/>
+      <c r="M43" s="197"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="197"/>
       <c r="B44" s="151"/>
       <c r="C44" s="151"/>
       <c r="D44" s="18">
@@ -5470,13 +5723,13 @@
       <c r="G44" s="151"/>
       <c r="H44" s="151"/>
       <c r="I44" s="65"/>
-      <c r="J44" s="193"/>
-      <c r="K44" s="193"/>
-      <c r="L44" s="193"/>
-      <c r="M44" s="193"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A45" s="193"/>
+      <c r="J44" s="197"/>
+      <c r="K44" s="197"/>
+      <c r="L44" s="197"/>
+      <c r="M44" s="197"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="197"/>
       <c r="B45" s="151"/>
       <c r="C45" s="151"/>
       <c r="D45" s="18">
@@ -5487,13 +5740,13 @@
       <c r="G45" s="151"/>
       <c r="H45" s="151"/>
       <c r="I45" s="65"/>
-      <c r="J45" s="193"/>
-      <c r="K45" s="193"/>
-      <c r="L45" s="193"/>
-      <c r="M45" s="193"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" s="193"/>
+      <c r="J45" s="197"/>
+      <c r="K45" s="197"/>
+      <c r="L45" s="197"/>
+      <c r="M45" s="197"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="197"/>
       <c r="B46" s="151"/>
       <c r="C46" s="151"/>
       <c r="D46" s="18">
@@ -5504,13 +5757,13 @@
       <c r="G46" s="151"/>
       <c r="H46" s="151"/>
       <c r="I46" s="153"/>
-      <c r="J46" s="193"/>
-      <c r="K46" s="193"/>
-      <c r="L46" s="193"/>
-      <c r="M46" s="193"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" s="195"/>
+      <c r="J46" s="197"/>
+      <c r="K46" s="197"/>
+      <c r="L46" s="197"/>
+      <c r="M46" s="197"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="199"/>
       <c r="B47" s="152"/>
       <c r="C47" s="152"/>
       <c r="D47" s="13">
@@ -5521,10 +5774,10 @@
       <c r="G47" s="152"/>
       <c r="H47" s="152"/>
       <c r="I47" s="152"/>
-      <c r="J47" s="195"/>
-      <c r="K47" s="195"/>
-      <c r="L47" s="195"/>
-      <c r="M47" s="195"/>
+      <c r="J47" s="199"/>
+      <c r="K47" s="199"/>
+      <c r="L47" s="199"/>
+      <c r="M47" s="199"/>
     </row>
   </sheetData>
   <mergeCells count="37">

</xml_diff>

<commit_message>
Bug fixes and update of excel input mask
</commit_message>
<xml_diff>
--- a/teaser/examples/2021-03-24_Hüllflächen_Zonen_Shells_of_Zones.xlsx
+++ b/teaser/examples/2021-03-24_Hüllflächen_Zonen_Shells_of_Zones.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EESchwimm\TEASER\teaser\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\TEASER\teaser\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC883A81-6CD2-48E7-BF83-F9810A7E3B07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hüllflächen, Himmelsricht." sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <definedName name="GlassA" localSheetId="1">[1]Dropdown!#REF!</definedName>
     <definedName name="GlassA">[1]Dropdown!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,191 +44,62 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={7F796FA0-45EC-4C4C-843B-360D0385E38E}</author>
-    <author>tc={F73AF337-B134-4C39-9107-82E90BF9956F}</author>
-    <author>tc={F4ECF03F-FA93-47D6-80B6-B15AA339D531}</author>
     <author>tc={E25679EC-AF68-49A1-8507-B6CF62C08D43}</author>
     <author>tc={EC0811A3-7202-47EB-9217-80E3351DF89A}</author>
-    <author>tc={7F1FE8C0-BC0B-4180-A6B6-22AF3675656E}</author>
     <author>tc={AFAD1E39-F4C4-4A33-952E-60446B18A8E1}</author>
-    <author>tc={243AE133-3DCA-48EA-A3CC-F3E7BB1287C4}</author>
     <author>tc={BB49A417-0C91-4FBA-A209-8C9D51A02D76}</author>
     <author>tc={E2D2AD93-2ABA-461B-840E-EE396FE1B71C}</author>
   </authors>
   <commentList>
-    <comment ref="J4" authorId="0" shapeId="0">
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Kommentarthread]
+        <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
-    Zone in Zone?
-Vorschlag: Wände zur Schwimmhalle als innere Wände addieren um Wärmekapazitäten zu berücksichtigen.</t>
-        </r>
+    Zone in Zone</t>
       </text>
     </comment>
-    <comment ref="V7" authorId="1" shapeId="0">
+    <comment ref="G13" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
-    enthält Wand zum Technikraum * 0,5</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V9" authorId="2" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
-    enthält Wand zum Technikraum * 0,5</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G13" authorId="3" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Kommentarthread]
+        <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     obere etage?</t>
-        </r>
       </text>
     </comment>
-    <comment ref="Q15" authorId="4" shapeId="0">
+    <comment ref="Q15" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Kommentarthread]
+        <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     enthählt Wände zum Erdbooden</t>
-        </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="5" shapeId="0">
+    <comment ref="Q16" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Kommentarthread]
+        <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
-    Innere Wände ohne Kontakt mit anderen Zonen 
-+ 
-(Innere Wände mit Kontakt mit anderen Zonen *0,5)</t>
-        </r>
+    enthählt wand zum schwimmbecken</t>
       </text>
     </comment>
-    <comment ref="Q16" authorId="6" shapeId="0">
+    <comment ref="G18" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
-    enthählt wand zum schwimmbecken(*0,5)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A18" authorId="7" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
-    Abhangdecken?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G18" authorId="8" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Kommentarthread]
+        <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     obere etage?</t>
-        </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="9" shapeId="0">
+    <comment ref="I19" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Kommentarthread]
+        <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     Ohne Wasserfläche</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -235,26 +107,17 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={B0FCD963-ED35-4353-B03A-99593B0E7AFB}</author>
   </authors>
   <commentList>
-    <comment ref="A41" authorId="0" shapeId="0">
+    <comment ref="A41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Kommentarthread]
+        <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     Horizontale Fenster werden in Teaser nicht erstellt</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -832,7 +695,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1681,7 +1544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2057,9 +1920,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2099,9 +1959,6 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2165,6 +2022,69 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2177,100 +2097,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -2605,14 +2465,7 @@
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="J4" dT="2021-03-04T10:38:49.81" personId="{06C71BA3-71A5-469C-81E3-2F24F58D5E9C}" id="{7F796FA0-45EC-4C4C-843B-360D0385E38E}">
-    <text>Zone in Zone?
-Vorschlag: Wände zur Schwimmhalle als innere Wände addieren um Wärmekapazitäten zu berücksichtigen.</text>
-  </threadedComment>
-  <threadedComment ref="V7" dT="2021-03-04T11:24:24.27" personId="{06C71BA3-71A5-469C-81E3-2F24F58D5E9C}" id="{F73AF337-B134-4C39-9107-82E90BF9956F}">
-    <text>enthält Wand zum Technikraum * 0,5</text>
-  </threadedComment>
-  <threadedComment ref="V9" dT="2021-03-04T11:24:24.27" personId="{06C71BA3-71A5-469C-81E3-2F24F58D5E9C}" id="{F4ECF03F-FA93-47D6-80B6-B15AA339D531}">
-    <text>enthält Wand zum Technikraum * 0,5</text>
+    <text>Zone in Zone</text>
   </threadedComment>
   <threadedComment ref="G13" dT="2021-03-04T10:12:37.44" personId="{06C71BA3-71A5-469C-81E3-2F24F58D5E9C}" id="{E25679EC-AF68-49A1-8507-B6CF62C08D43}">
     <text>obere etage?</text>
@@ -2620,16 +2473,8 @@
   <threadedComment ref="Q15" dT="2021-03-04T11:03:51.01" personId="{06C71BA3-71A5-469C-81E3-2F24F58D5E9C}" id="{EC0811A3-7202-47EB-9217-80E3351DF89A}">
     <text>enthählt Wände zum Erdbooden</text>
   </threadedComment>
-  <threadedComment ref="A16" dT="2021-03-04T10:40:21.15" personId="{06C71BA3-71A5-469C-81E3-2F24F58D5E9C}" id="{7F1FE8C0-BC0B-4180-A6B6-22AF3675656E}">
-    <text>Innere Wände ohne Kontakt mit anderen Zonen 
-+ 
-(Innere Wände mit Kontakt mit anderen Zonen *0,5)</text>
-  </threadedComment>
   <threadedComment ref="Q16" dT="2021-03-04T11:04:59.57" personId="{06C71BA3-71A5-469C-81E3-2F24F58D5E9C}" id="{AFAD1E39-F4C4-4A33-952E-60446B18A8E1}">
-    <text>enthählt wand zum schwimmbecken(*0,5)</text>
-  </threadedComment>
-  <threadedComment ref="A18" dT="2021-03-04T10:13:03.98" personId="{06C71BA3-71A5-469C-81E3-2F24F58D5E9C}" id="{243AE133-3DCA-48EA-A3CC-F3E7BB1287C4}">
-    <text>Abhangdecken?</text>
+    <text>enthählt wand zum schwimmbecken</text>
   </threadedComment>
   <threadedComment ref="G18" dT="2021-03-04T10:16:23.76" personId="{06C71BA3-71A5-469C-81E3-2F24F58D5E9C}" id="{BB49A417-0C91-4FBA-A209-8C9D51A02D76}">
     <text>obere etage?</text>
@@ -2649,72 +2494,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5:AD13"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="36" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="36" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="25"/>
-    <col min="6" max="6" width="13.28515625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="36" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="36" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="25"/>
+    <col min="6" max="6" width="13.33203125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="25" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="25"/>
-    <col min="10" max="10" width="11.42578125" style="25" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" style="25" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="25"/>
-    <col min="14" max="14" width="7.7109375" style="25" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="25"/>
-    <col min="16" max="16" width="7.7109375" style="25" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" style="25"/>
-    <col min="18" max="18" width="26.28515625" style="25" customWidth="1"/>
-    <col min="19" max="19" width="22.28515625" style="25" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" style="25" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="25" customWidth="1"/>
-    <col min="22" max="22" width="26.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="25"/>
+    <col min="10" max="10" width="11.44140625" style="25" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" style="25" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" style="25"/>
+    <col min="14" max="14" width="7.6640625" style="25" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" style="25"/>
+    <col min="16" max="16" width="7.6640625" style="25" customWidth="1"/>
+    <col min="17" max="17" width="11.44140625" style="25"/>
+    <col min="18" max="18" width="26.33203125" style="25" customWidth="1"/>
+    <col min="19" max="19" width="22.33203125" style="25" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" style="25" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="25" customWidth="1"/>
+    <col min="22" max="22" width="26.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" style="25" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="29" style="25" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="18.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="11.42578125" style="25"/>
+    <col min="28" max="30" width="18.44140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="11.44140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="191" t="s">
+    <row r="1" spans="1:31" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="192"/>
-      <c r="C1" s="192"/>
-      <c r="D1" s="192"/>
-      <c r="E1" s="192"/>
-      <c r="F1" s="192"/>
-      <c r="G1" s="192"/>
-      <c r="H1" s="192"/>
-      <c r="I1" s="192"/>
-      <c r="J1" s="192"/>
-      <c r="K1" s="192"/>
-      <c r="L1" s="192"/>
-      <c r="M1" s="192"/>
-      <c r="N1" s="192"/>
-      <c r="O1" s="192"/>
-      <c r="P1" s="192"/>
-      <c r="Q1" s="192"/>
-    </row>
-    <row r="2" spans="1:31" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="168"/>
+      <c r="G1" s="168"/>
+      <c r="H1" s="168"/>
+      <c r="I1" s="168"/>
+      <c r="J1" s="168"/>
+      <c r="K1" s="168"/>
+      <c r="L1" s="168"/>
+      <c r="M1" s="168"/>
+      <c r="N1" s="168"/>
+      <c r="O1" s="168"/>
+      <c r="P1" s="168"/>
+      <c r="Q1" s="168"/>
+    </row>
+    <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="40"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -2733,146 +2578,146 @@
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
     </row>
-    <row r="3" spans="1:31" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="26"/>
-      <c r="B3" s="185" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="186"/>
-      <c r="D3" s="187" t="s">
+      <c r="B3" s="186" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="179"/>
+      <c r="D3" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="188"/>
-      <c r="F3" s="189" t="s">
+      <c r="E3" s="177"/>
+      <c r="F3" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="186"/>
-      <c r="H3" s="195" t="s">
+      <c r="G3" s="179"/>
+      <c r="H3" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="188"/>
-      <c r="J3" s="189" t="s">
+      <c r="I3" s="177"/>
+      <c r="J3" s="178" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="186"/>
-      <c r="L3" s="193" t="s">
+      <c r="K3" s="179"/>
+      <c r="L3" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="194"/>
-      <c r="N3" s="193" t="s">
+      <c r="M3" s="174"/>
+      <c r="N3" s="173" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="194"/>
-      <c r="P3" s="187" t="s">
+      <c r="O3" s="174"/>
+      <c r="P3" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="187"/>
-      <c r="S3" s="169" t="s">
+      <c r="Q3" s="175"/>
+      <c r="S3" s="188" t="s">
         <v>46</v>
       </c>
-      <c r="T3" s="170"/>
-      <c r="U3" s="163" t="s">
+      <c r="T3" s="189"/>
+      <c r="U3" s="161" t="s">
         <v>58</v>
       </c>
-      <c r="V3" s="164" t="s">
+      <c r="V3" s="162" t="s">
         <v>57</v>
       </c>
-      <c r="W3" s="164" t="s">
+      <c r="W3" s="162" t="s">
         <v>56</v>
       </c>
-      <c r="X3" s="164" t="s">
+      <c r="X3" s="162" t="s">
         <v>55</v>
       </c>
-      <c r="Y3" s="164" t="s">
+      <c r="Y3" s="162" t="s">
         <v>54</v>
       </c>
-      <c r="Z3" s="164" t="s">
+      <c r="Z3" s="162" t="s">
         <v>53</v>
       </c>
-      <c r="AA3" s="164" t="s">
+      <c r="AA3" s="162" t="s">
         <v>65</v>
       </c>
-      <c r="AB3" s="164" t="s">
+      <c r="AB3" s="162" t="s">
         <v>66</v>
       </c>
-      <c r="AC3" s="164" t="s">
+      <c r="AC3" s="162" t="s">
         <v>67</v>
       </c>
-      <c r="AD3" s="164" t="s">
+      <c r="AD3" s="162" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="190" t="s">
+      <c r="B4" s="172" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="174"/>
-      <c r="D4" s="173" t="s">
+      <c r="C4" s="187"/>
+      <c r="D4" s="171" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="174"/>
-      <c r="F4" s="173" t="s">
+      <c r="E4" s="187"/>
+      <c r="F4" s="171" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="174"/>
-      <c r="H4" s="173" t="s">
+      <c r="G4" s="187"/>
+      <c r="H4" s="171" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="174"/>
-      <c r="J4" s="175" t="s">
+      <c r="I4" s="187"/>
+      <c r="J4" s="192" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="176"/>
-      <c r="L4" s="177" t="s">
+      <c r="K4" s="193"/>
+      <c r="L4" s="169" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="178"/>
-      <c r="N4" s="177" t="s">
+      <c r="M4" s="170"/>
+      <c r="N4" s="169" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="178"/>
-      <c r="P4" s="173" t="s">
+      <c r="O4" s="170"/>
+      <c r="P4" s="171" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="190"/>
-      <c r="S4" s="171"/>
-      <c r="T4" s="172"/>
+      <c r="Q4" s="172"/>
+      <c r="S4" s="190"/>
+      <c r="T4" s="191"/>
       <c r="U4" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="V4" s="162" t="s">
+      <c r="V4" s="160" t="s">
         <v>48</v>
       </c>
-      <c r="W4" s="162" t="s">
+      <c r="W4" s="160" t="s">
         <v>49</v>
       </c>
-      <c r="X4" s="162" t="s">
+      <c r="X4" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="Y4" s="162" t="s">
+      <c r="Y4" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="Z4" s="162" t="s">
+      <c r="Z4" s="160" t="s">
         <v>52</v>
       </c>
-      <c r="AA4" s="162" t="s">
+      <c r="AA4" s="160" t="s">
         <v>117</v>
       </c>
-      <c r="AB4" s="162" t="s">
+      <c r="AB4" s="160" t="s">
         <v>118</v>
       </c>
-      <c r="AC4" s="162" t="s">
+      <c r="AC4" s="160" t="s">
         <v>119</v>
       </c>
-      <c r="AD4" s="162" t="s">
+      <c r="AD4" s="160" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="179" t="s">
+    <row r="5" spans="1:31" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="180" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2928,11 +2773,11 @@
       <c r="T5" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="U5" s="146">
+      <c r="U5" s="145">
         <f t="shared" ref="U5:U10" si="0">SUM(V5:AD5)</f>
         <v>552.79999999999995</v>
       </c>
-      <c r="V5" s="144">
+      <c r="V5" s="143">
         <f>25*16.66</f>
         <v>416.5</v>
       </c>
@@ -2942,7 +2787,7 @@
       <c r="X5" s="57">
         <v>0</v>
       </c>
-      <c r="Y5" s="145">
+      <c r="Y5" s="144">
         <v>136.30000000000001</v>
       </c>
       <c r="Z5" s="57">
@@ -2961,8 +2806,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="180"/>
+    <row r="6" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="181"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -3009,17 +2854,17 @@
       <c r="Q6" s="89">
         <v>0</v>
       </c>
-      <c r="S6" s="143" t="s">
+      <c r="S6" s="142" t="s">
         <v>105</v>
       </c>
       <c r="T6" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="U6" s="146">
+      <c r="U6" s="145">
         <f t="shared" si="0"/>
         <v>543.43000000000006</v>
       </c>
-      <c r="V6" s="144">
+      <c r="V6" s="143">
         <f>25*16.66</f>
         <v>416.5</v>
       </c>
@@ -3029,7 +2874,7 @@
       <c r="X6" s="58">
         <v>0</v>
       </c>
-      <c r="Y6" s="145">
+      <c r="Y6" s="144">
         <v>126.93</v>
       </c>
       <c r="Z6" s="58">
@@ -3049,8 +2894,8 @@
       </c>
       <c r="AE6" s="132"/>
     </row>
-    <row r="7" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="180"/>
+    <row r="7" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="181"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -3096,17 +2941,17 @@
       <c r="Q7" s="89">
         <v>0</v>
       </c>
-      <c r="S7" s="143" t="s">
+      <c r="S7" s="142" t="s">
         <v>106</v>
       </c>
       <c r="T7" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="U7" s="146">
+      <c r="U7" s="145">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V7" s="147">
+      <c r="V7" s="201">
         <v>0</v>
       </c>
       <c r="W7" s="58">
@@ -3115,7 +2960,7 @@
       <c r="X7" s="58">
         <v>0</v>
       </c>
-      <c r="Y7" s="145">
+      <c r="Y7" s="144">
         <v>0</v>
       </c>
       <c r="Z7" s="58">
@@ -3134,8 +2979,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="181"/>
+    <row r="8" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="182"/>
       <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3182,17 +3027,17 @@
         <f>6.25*5+3*3.25</f>
         <v>41</v>
       </c>
-      <c r="S8" s="143" t="s">
+      <c r="S8" s="142" t="s">
         <v>107</v>
       </c>
       <c r="T8" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="U8" s="146">
+      <c r="U8" s="145">
         <f t="shared" si="0"/>
         <v>183.666</v>
       </c>
-      <c r="V8" s="145">
+      <c r="V8" s="144">
         <v>146.52000000000001</v>
       </c>
       <c r="W8" s="58">
@@ -3201,7 +3046,7 @@
       <c r="X8" s="58">
         <v>0</v>
       </c>
-      <c r="Y8" s="145">
+      <c r="Y8" s="144">
         <v>37.146000000000001</v>
       </c>
       <c r="Z8" s="58">
@@ -3220,8 +3065,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="182" t="s">
+    <row r="9" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="183" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -3271,18 +3116,18 @@
         <f>1.51*2+2*1.51</f>
         <v>6.04</v>
       </c>
-      <c r="S9" s="143" t="s">
+      <c r="S9" s="142" t="s">
         <v>108</v>
       </c>
       <c r="T9" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="U9" s="146">
+      <c r="U9" s="145">
         <f t="shared" si="0"/>
-        <v>43.316000000000003</v>
-      </c>
-      <c r="V9" s="147">
-        <v>43.316000000000003</v>
+        <v>86</v>
+      </c>
+      <c r="V9" s="201">
+        <v>86</v>
       </c>
       <c r="W9" s="58">
         <v>0</v>
@@ -3290,7 +3135,7 @@
       <c r="X9" s="58">
         <v>0</v>
       </c>
-      <c r="Y9" s="145">
+      <c r="Y9" s="144">
         <v>0</v>
       </c>
       <c r="Z9" s="58">
@@ -3308,12 +3153,12 @@
       <c r="AD9" s="58">
         <v>0</v>
       </c>
-      <c r="AE9" s="155" t="s">
+      <c r="AE9" s="153" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="183"/>
+    <row r="10" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="184"/>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -3365,11 +3210,11 @@
       <c r="T10" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="U10" s="146">
+      <c r="U10" s="145">
         <f t="shared" si="0"/>
         <v>1069.7560000000001</v>
       </c>
-      <c r="V10" s="145">
+      <c r="V10" s="144">
         <v>942.95600000000002</v>
       </c>
       <c r="W10" s="58">
@@ -3378,7 +3223,7 @@
       <c r="X10" s="58">
         <v>0</v>
       </c>
-      <c r="Y10" s="145">
+      <c r="Y10" s="144">
         <v>126.8</v>
       </c>
       <c r="Z10" s="58">
@@ -3398,8 +3243,8 @@
       </c>
       <c r="AE10" s="47"/>
     </row>
-    <row r="11" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="183"/>
+    <row r="11" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="184"/>
       <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
@@ -3451,7 +3296,7 @@
       <c r="T11" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="U11" s="146"/>
+      <c r="U11" s="145"/>
       <c r="V11" s="58">
         <v>301.14999999999998</v>
       </c>
@@ -3481,8 +3326,8 @@
       </c>
       <c r="AE11" s="47"/>
     </row>
-    <row r="12" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="184"/>
+    <row r="12" spans="1:31" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="185"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -3535,7 +3380,7 @@
       <c r="T12" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="U12" s="146"/>
+      <c r="U12" s="145"/>
       <c r="V12" s="58">
         <f>2*25+2*16.66</f>
         <v>83.32</v>
@@ -3567,7 +3412,7 @@
       </c>
       <c r="AE12" s="47"/>
     </row>
-    <row r="13" spans="1:31" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
         <v>42</v>
       </c>
@@ -3582,7 +3427,7 @@
         <v>267.75</v>
       </c>
       <c r="F13" s="106"/>
-      <c r="G13" s="136">
+      <c r="G13" s="135">
         <f>8*31.5</f>
         <v>252</v>
       </c>
@@ -3611,7 +3456,7 @@
       <c r="T13" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="U13" s="146"/>
+      <c r="U13" s="145"/>
       <c r="V13" s="58">
         <f>IF(V5&gt;0,V10/V5,0)</f>
         <v>2.2640000000000002</v>
@@ -3648,11 +3493,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE13" s="155" t="s">
+      <c r="AE13" s="153" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>17</v>
       </c>
@@ -3687,39 +3532,39 @@
       <c r="S14" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="T14" s="160" t="s">
+      <c r="T14" s="158" t="s">
         <v>125</v>
       </c>
-      <c r="U14" s="146"/>
-      <c r="V14" s="159">
+      <c r="U14" s="145"/>
+      <c r="V14" s="157">
         <v>2</v>
       </c>
-      <c r="W14" s="159">
-        <v>0</v>
-      </c>
-      <c r="X14" s="159">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="159">
+      <c r="W14" s="157">
+        <v>0</v>
+      </c>
+      <c r="X14" s="157">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="157">
         <v>2</v>
       </c>
-      <c r="Z14" s="159">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="159">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="159">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="159">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Z14" s="157">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="157">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="157">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="157">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29" t="s">
         <v>90</v>
       </c>
@@ -3752,7 +3597,7 @@
       <c r="N15" s="109"/>
       <c r="O15" s="110"/>
       <c r="P15" s="111"/>
-      <c r="Q15" s="142">
+      <c r="Q15" s="141">
         <f>17.2*8+9.26*25+2.23*(25+9.26+9.26)</f>
         <v>466.14960000000002</v>
       </c>
@@ -3760,10 +3605,10 @@
       <c r="S15" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="T15" s="160" t="s">
+      <c r="T15" s="158" t="s">
         <v>102</v>
       </c>
-      <c r="U15" s="146"/>
+      <c r="U15" s="145"/>
       <c r="V15" s="58" t="s">
         <v>135</v>
       </c>
@@ -3792,31 +3637,31 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="133" t="s">
+    <row r="16" spans="1:31" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="137"/>
+      <c r="B16" s="136"/>
       <c r="C16" s="121">
-        <f>6.2*((C17/8.51)*0.5+8.51*0.5+8.51) + 6.2*(3.885+5.165)</f>
-        <v>225.04735957696826</v>
-      </c>
-      <c r="D16" s="138"/>
+        <f>6.2*((C17/8.51)+8.51+8.51) + 6.2*(3.885+5.165)</f>
+        <v>341.22271915393657</v>
+      </c>
+      <c r="D16" s="137"/>
       <c r="E16" s="121">
-        <f>(31.5*0.5+8.5)*3.25</f>
-        <v>78.8125</v>
-      </c>
-      <c r="F16" s="139"/>
+        <f>(31.5+8.5)*3.25</f>
+        <v>130</v>
+      </c>
+      <c r="F16" s="138"/>
       <c r="G16" s="121">
         <f>3.25*(31.5+8+8+(7*8)+(2*8))</f>
         <v>388.375</v>
       </c>
-      <c r="H16" s="139"/>
+      <c r="H16" s="138"/>
       <c r="I16" s="121">
-        <f>6.2*(25*0.5+43*0.5+14)</f>
-        <v>297.60000000000002</v>
-      </c>
-      <c r="J16" s="139"/>
+        <f>6.2*(25+43+14)</f>
+        <v>508.40000000000003</v>
+      </c>
+      <c r="J16" s="138"/>
       <c r="K16" s="121">
         <f>(21.2/2)*4*3.25</f>
         <v>137.79999999999998</v>
@@ -3825,10 +3670,10 @@
       <c r="M16" s="110"/>
       <c r="N16" s="109"/>
       <c r="O16" s="110"/>
-      <c r="P16" s="140"/>
-      <c r="Q16" s="135">
-        <f>0.5*16.66*2.23+(25-16.66)*2.23+17.2*6.25+8*6.25*2</f>
-        <v>244.67410000000001</v>
+      <c r="P16" s="139"/>
+      <c r="Q16" s="134">
+        <f>16.66*2.23+(25-16.66)*2.23+17.2*6.25+8*6.25*2</f>
+        <v>263.25</v>
       </c>
       <c r="S16" s="51" t="s">
         <v>101</v>
@@ -3836,7 +3681,7 @@
       <c r="T16" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="U16" s="146"/>
+      <c r="U16" s="145"/>
       <c r="V16" s="58" t="s">
         <v>122</v>
       </c>
@@ -3865,7 +3710,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:32" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29" t="s">
         <v>45</v>
       </c>
@@ -3910,7 +3755,7 @@
       <c r="T17" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="U17" s="146"/>
+      <c r="U17" s="145"/>
       <c r="V17" s="58" t="s">
         <v>121</v>
       </c>
@@ -3939,28 +3784,28 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="133" t="s">
+    <row r="18" spans="1:32" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="137"/>
+      <c r="B18" s="136"/>
       <c r="C18" s="121">
         <v>0</v>
       </c>
-      <c r="D18" s="138"/>
+      <c r="D18" s="137"/>
       <c r="E18" s="121">
         <v>0</v>
       </c>
-      <c r="F18" s="139"/>
-      <c r="G18" s="134">
+      <c r="F18" s="138"/>
+      <c r="G18" s="133">
         <f>8*31.5</f>
         <v>252</v>
       </c>
-      <c r="H18" s="139"/>
+      <c r="H18" s="138"/>
       <c r="I18" s="121">
         <v>0</v>
       </c>
-      <c r="J18" s="139"/>
+      <c r="J18" s="138"/>
       <c r="K18" s="121">
         <f>11.79+9.41</f>
         <v>21.2</v>
@@ -3969,8 +3814,8 @@
       <c r="M18" s="110"/>
       <c r="N18" s="109"/>
       <c r="O18" s="118"/>
-      <c r="P18" s="140"/>
-      <c r="Q18" s="141">
+      <c r="P18" s="139"/>
+      <c r="Q18" s="140">
         <f>25*9.26</f>
         <v>231.5</v>
       </c>
@@ -3981,7 +3826,7 @@
       <c r="T18" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="U18" s="146"/>
+      <c r="U18" s="145"/>
       <c r="V18" s="58" t="s">
         <v>112</v>
       </c>
@@ -4010,7 +3855,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:32" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:32" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="37" t="s">
         <v>88</v>
       </c>
@@ -4027,7 +3872,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="116"/>
-      <c r="I19" s="134">
+      <c r="I19" s="133">
         <f>9.26*25</f>
         <v>231.5</v>
       </c>
@@ -4051,37 +3896,37 @@
       <c r="T19" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="U19" s="146"/>
-      <c r="V19" s="145">
+      <c r="U19" s="145"/>
+      <c r="V19" s="144">
         <v>0.8</v>
       </c>
-      <c r="W19" s="145">
-        <v>0</v>
-      </c>
-      <c r="X19" s="145">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="145">
+      <c r="W19" s="144">
+        <v>0</v>
+      </c>
+      <c r="X19" s="144">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="144">
         <v>0.8</v>
       </c>
-      <c r="Z19" s="145">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="145">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="145">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="145">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="145">
-        <v>0</v>
-      </c>
-      <c r="AF19" s="161"/>
-    </row>
-    <row r="20" spans="1:32" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Z19" s="144">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="144">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="144">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="144">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="144">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="159"/>
+    </row>
+    <row r="20" spans="1:32" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>18</v>
       </c>
@@ -4125,41 +3970,41 @@
       <c r="T20" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="U20" s="146"/>
-      <c r="V20" s="145">
+      <c r="U20" s="145"/>
+      <c r="V20" s="144">
         <v>30</v>
       </c>
-      <c r="W20" s="145">
-        <v>0</v>
-      </c>
-      <c r="X20" s="145">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="145">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="145">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="145">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="145">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="145">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="145">
-        <v>0</v>
-      </c>
-      <c r="AF20" s="161"/>
-    </row>
-    <row r="21" spans="1:32" ht="58.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="156"/>
-      <c r="B21" s="156"/>
+      <c r="W20" s="144">
+        <v>0</v>
+      </c>
+      <c r="X20" s="144">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="144">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="144">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="144">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="144">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="144">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="144">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="159"/>
+    </row>
+    <row r="21" spans="1:32" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="154"/>
+      <c r="B21" s="154"/>
       <c r="C21" s="38"/>
-      <c r="D21" s="156"/>
+      <c r="D21" s="154"/>
       <c r="E21" s="38"/>
       <c r="F21" s="39"/>
       <c r="G21" s="38"/>
@@ -4180,7 +4025,7 @@
       <c r="T21" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="U21" s="146"/>
+      <c r="U21" s="145"/>
       <c r="V21" s="58" t="s">
         <v>113</v>
       </c>
@@ -4208,79 +4053,79 @@
       <c r="AD21" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="AF21" s="161"/>
-    </row>
-    <row r="22" spans="1:32" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="158"/>
-      <c r="B22" s="158"/>
-      <c r="C22" s="158"/>
-      <c r="D22" s="158"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158"/>
-      <c r="J22" s="158"/>
-      <c r="K22" s="158"/>
-      <c r="L22" s="158"/>
-      <c r="M22" s="158"/>
-      <c r="N22" s="158"/>
-      <c r="O22" s="158"/>
-      <c r="P22" s="158"/>
+      <c r="AF21" s="159"/>
+    </row>
+    <row r="22" spans="1:32" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="156"/>
+      <c r="B22" s="156"/>
+      <c r="C22" s="156"/>
+      <c r="D22" s="156"/>
+      <c r="E22" s="156"/>
+      <c r="F22" s="156"/>
+      <c r="G22" s="156"/>
+      <c r="H22" s="156"/>
+      <c r="I22" s="156"/>
+      <c r="J22" s="156"/>
+      <c r="K22" s="156"/>
+      <c r="L22" s="156"/>
+      <c r="M22" s="156"/>
+      <c r="N22" s="156"/>
+      <c r="O22" s="156"/>
+      <c r="P22" s="156"/>
       <c r="Q22" s="38"/>
       <c r="S22" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="T22" s="160" t="s">
+      <c r="T22" s="158" t="s">
         <v>132</v>
       </c>
-      <c r="U22" s="146"/>
-      <c r="V22" s="159">
+      <c r="U22" s="145"/>
+      <c r="V22" s="157">
         <v>30</v>
       </c>
-      <c r="W22" s="159">
-        <v>0</v>
-      </c>
-      <c r="X22" s="159">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="159">
+      <c r="W22" s="157">
+        <v>0</v>
+      </c>
+      <c r="X22" s="157">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="157">
         <v>30</v>
       </c>
-      <c r="Z22" s="159">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="159">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="159">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="159">
-        <v>0</v>
-      </c>
-      <c r="AD22" s="159">
-        <v>0</v>
-      </c>
-      <c r="AF22" s="161"/>
-    </row>
-    <row r="23" spans="1:32" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z22" s="157">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="157">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="157">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="157">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="157">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="159"/>
+    </row>
+    <row r="23" spans="1:32" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="40"/>
-      <c r="B23" s="157"/>
-      <c r="C23" s="157"/>
-      <c r="D23" s="157"/>
-      <c r="E23" s="157"/>
-      <c r="F23" s="157"/>
-      <c r="G23" s="157"/>
-      <c r="H23" s="157"/>
-      <c r="I23" s="157"/>
-      <c r="J23" s="157"/>
-      <c r="K23" s="157"/>
-      <c r="L23" s="157"/>
-      <c r="M23" s="157"/>
-      <c r="N23" s="157"/>
-      <c r="O23" s="157"/>
-      <c r="P23" s="157"/>
+      <c r="B23" s="155"/>
+      <c r="C23" s="155"/>
+      <c r="D23" s="155"/>
+      <c r="E23" s="155"/>
+      <c r="F23" s="155"/>
+      <c r="G23" s="155"/>
+      <c r="H23" s="155"/>
+      <c r="I23" s="155"/>
+      <c r="J23" s="155"/>
+      <c r="K23" s="155"/>
+      <c r="L23" s="155"/>
+      <c r="M23" s="155"/>
+      <c r="N23" s="155"/>
+      <c r="O23" s="155"/>
+      <c r="P23" s="155"/>
       <c r="Q23" s="38"/>
       <c r="S23" s="51" t="s">
         <v>110</v>
@@ -4288,7 +4133,7 @@
       <c r="T23" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="U23" s="146"/>
+      <c r="U23" s="145"/>
       <c r="V23" s="58" t="s">
         <v>112</v>
       </c>
@@ -4316,25 +4161,25 @@
       <c r="AD23" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="AF23" s="161"/>
-    </row>
-    <row r="24" spans="1:32" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF23" s="159"/>
+    </row>
+    <row r="24" spans="1:32" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="40"/>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="157"/>
-      <c r="I24" s="157"/>
-      <c r="J24" s="157"/>
-      <c r="K24" s="157"/>
-      <c r="L24" s="157"/>
-      <c r="M24" s="157"/>
-      <c r="N24" s="157"/>
-      <c r="O24" s="157"/>
-      <c r="P24" s="157"/>
+      <c r="B24" s="155"/>
+      <c r="C24" s="155"/>
+      <c r="D24" s="155"/>
+      <c r="E24" s="155"/>
+      <c r="F24" s="155"/>
+      <c r="G24" s="155"/>
+      <c r="H24" s="155"/>
+      <c r="I24" s="155"/>
+      <c r="J24" s="155"/>
+      <c r="K24" s="155"/>
+      <c r="L24" s="155"/>
+      <c r="M24" s="155"/>
+      <c r="N24" s="155"/>
+      <c r="O24" s="155"/>
+      <c r="P24" s="155"/>
       <c r="Q24" s="38"/>
       <c r="S24" s="51" t="s">
         <v>126</v>
@@ -4342,7 +4187,7 @@
       <c r="T24" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="U24" s="146"/>
+      <c r="U24" s="145"/>
       <c r="V24" s="58" t="s">
         <v>113</v>
       </c>
@@ -4371,23 +4216,23 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:32" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="40"/>
-      <c r="B25" s="157"/>
-      <c r="C25" s="157"/>
-      <c r="D25" s="157"/>
-      <c r="E25" s="157"/>
-      <c r="F25" s="157"/>
-      <c r="G25" s="157"/>
-      <c r="H25" s="157"/>
-      <c r="I25" s="157"/>
-      <c r="J25" s="157"/>
-      <c r="K25" s="157"/>
-      <c r="L25" s="157"/>
-      <c r="M25" s="157"/>
-      <c r="N25" s="157"/>
-      <c r="O25" s="157"/>
-      <c r="P25" s="157"/>
+      <c r="B25" s="155"/>
+      <c r="C25" s="155"/>
+      <c r="D25" s="155"/>
+      <c r="E25" s="155"/>
+      <c r="F25" s="155"/>
+      <c r="G25" s="155"/>
+      <c r="H25" s="155"/>
+      <c r="I25" s="155"/>
+      <c r="J25" s="155"/>
+      <c r="K25" s="155"/>
+      <c r="L25" s="155"/>
+      <c r="M25" s="155"/>
+      <c r="N25" s="155"/>
+      <c r="O25" s="155"/>
+      <c r="P25" s="155"/>
       <c r="Q25" s="38"/>
       <c r="S25" s="51" t="s">
         <v>127</v>
@@ -4395,7 +4240,7 @@
       <c r="T25" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="U25" s="146"/>
+      <c r="U25" s="145"/>
       <c r="V25" s="58">
         <v>0</v>
       </c>
@@ -4424,14 +4269,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:32" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="S26" s="51" t="s">
         <v>128</v>
       </c>
       <c r="T26" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="U26" s="146"/>
+      <c r="U26" s="145"/>
       <c r="V26" s="58">
         <v>0</v>
       </c>
@@ -4460,12 +4305,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:32" ht="43.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:32" ht="46.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:32" ht="44.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:32" ht="46.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:32" ht="43.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:32" ht="46.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:32" ht="44.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:32" ht="46.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="P4:Q4"/>
@@ -4474,19 +4332,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
   </mergeCells>
   <conditionalFormatting sqref="B23">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
@@ -4504,16 +4349,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V18:AD18 V21:AD21 V23:AD24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V18:AD18 V21:AD21 V23:AD24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"True, False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V16:AD16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V16:AD16" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ohne Ozon, mit Ozon, mit Ultrafiltration, mit Brom"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V15:AD15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V15:AD15" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Aktivkohlefilter mit Ozon, geschlossener Schnellfilter, geschlossener Sorptionsfilter, offener Schnellfilter, offener Saugfilter, Quantozonfilter, Quarzkiesfilter, Zweischichtfilter, Zweischichtfilter mit Ozon"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V17:AD17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V17:AD17" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Salzwasser, Süßwasser"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4528,7 +4373,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:U47"/>
   <sheetViews>
@@ -4536,35 +4381,35 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="8" customWidth="1"/>
-    <col min="2" max="3" width="16.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="43" customWidth="1"/>
-    <col min="6" max="6" width="46.85546875" style="8" customWidth="1"/>
-    <col min="7" max="8" width="27.140625" style="54" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" style="8" customWidth="1"/>
+    <col min="2" max="3" width="16.88671875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="46.88671875" style="8" customWidth="1"/>
+    <col min="7" max="8" width="27.109375" style="54" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" style="8" customWidth="1"/>
     <col min="10" max="10" width="0" style="8" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="8" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" style="8" hidden="1" customWidth="1"/>
     <col min="12" max="13" width="0" style="8" hidden="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="8"/>
+    <col min="14" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="200" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="199" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
       <c r="E1" s="44"/>
       <c r="F1" s="14"/>
       <c r="G1" s="55"/>
       <c r="H1" s="55"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:21" s="23" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="23" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>19</v>
       </c>
@@ -4592,20 +4437,20 @@
       <c r="I2" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="149" t="s">
+      <c r="J2" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="149" t="s">
+      <c r="K2" s="147" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="149" t="s">
+      <c r="L2" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="149" t="s">
+      <c r="M2" s="147" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -4630,8 +4475,8 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="201" t="s">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="200" t="s">
         <v>69</v>
       </c>
       <c r="B4" s="46"/>
@@ -4682,7 +4527,7 @@
         <v>0.77584580000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="198"/>
       <c r="B5" s="46"/>
       <c r="C5" s="46"/>
@@ -4724,7 +4569,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="198"/>
       <c r="B6" s="46"/>
       <c r="C6" s="46"/>
@@ -4766,7 +4611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="198"/>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
@@ -4808,7 +4653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="198"/>
       <c r="B8" s="46"/>
       <c r="C8" s="46"/>
@@ -4820,8 +4665,8 @@
       <c r="L8" s="198"/>
       <c r="M8" s="198"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="199"/>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="196"/>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="13">
@@ -4829,13 +4674,13 @@
       </c>
       <c r="H9" s="55"/>
       <c r="I9" s="55"/>
-      <c r="J9" s="199"/>
-      <c r="K9" s="199"/>
-      <c r="L9" s="199"/>
-      <c r="M9" s="199"/>
-    </row>
-    <row r="10" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="196" t="s">
+      <c r="J9" s="196"/>
+      <c r="K9" s="196"/>
+      <c r="L9" s="196"/>
+      <c r="M9" s="196"/>
+    </row>
+    <row r="10" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="194" t="s">
         <v>70</v>
       </c>
       <c r="B10" s="41"/>
@@ -4852,26 +4697,26 @@
       <c r="G10" s="52"/>
       <c r="H10" s="52"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="196" t="s">
+      <c r="J10" s="194" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="196" t="s">
+      <c r="K10" s="194" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="196" t="s">
+      <c r="L10" s="194" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="196" t="s">
+      <c r="M10" s="194" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="202" t="s">
+      <c r="N10" s="197" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="202"/>
-      <c r="P10" s="202"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="197"/>
+      <c r="O10" s="197"/>
+      <c r="P10" s="197"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="195"/>
       <c r="B11" s="42"/>
       <c r="C11" s="53"/>
       <c r="D11" s="18">
@@ -4886,16 +4731,16 @@
       <c r="G11" s="53"/>
       <c r="H11" s="53"/>
       <c r="I11" s="12"/>
-      <c r="J11" s="197"/>
-      <c r="K11" s="197"/>
-      <c r="L11" s="197"/>
-      <c r="M11" s="197"/>
-      <c r="N11" s="202"/>
-      <c r="O11" s="202"/>
-      <c r="P11" s="202"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="197"/>
+      <c r="J11" s="195"/>
+      <c r="K11" s="195"/>
+      <c r="L11" s="195"/>
+      <c r="M11" s="195"/>
+      <c r="N11" s="197"/>
+      <c r="O11" s="197"/>
+      <c r="P11" s="197"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="195"/>
       <c r="B12" s="42"/>
       <c r="C12" s="53"/>
       <c r="D12" s="12">
@@ -4912,12 +4757,12 @@
       <c r="K12" s="198"/>
       <c r="L12" s="198"/>
       <c r="M12" s="198"/>
-      <c r="N12" s="202"/>
-      <c r="O12" s="202"/>
-      <c r="P12" s="202"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="197"/>
+      <c r="N12" s="197"/>
+      <c r="O12" s="197"/>
+      <c r="P12" s="197"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="195"/>
       <c r="B13" s="42"/>
       <c r="C13" s="53"/>
       <c r="D13" s="12">
@@ -4932,12 +4777,12 @@
       <c r="K13" s="198"/>
       <c r="L13" s="198"/>
       <c r="M13" s="198"/>
-      <c r="N13" s="202"/>
-      <c r="O13" s="202"/>
-      <c r="P13" s="202"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="197"/>
+      <c r="N13" s="197"/>
+      <c r="O13" s="197"/>
+      <c r="P13" s="197"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="195"/>
       <c r="B14" s="53"/>
       <c r="C14" s="53"/>
       <c r="D14" s="12">
@@ -4952,12 +4797,12 @@
       <c r="K14" s="198"/>
       <c r="L14" s="198"/>
       <c r="M14" s="198"/>
-      <c r="N14" s="202"/>
-      <c r="O14" s="202"/>
-      <c r="P14" s="202"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="199"/>
+      <c r="N14" s="197"/>
+      <c r="O14" s="197"/>
+      <c r="P14" s="197"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="196"/>
       <c r="B15" s="44"/>
       <c r="C15" s="55"/>
       <c r="D15" s="13">
@@ -4968,16 +4813,16 @@
       <c r="G15" s="53"/>
       <c r="H15" s="55"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="199"/>
-      <c r="K15" s="199"/>
-      <c r="L15" s="199"/>
-      <c r="M15" s="199"/>
-      <c r="N15" s="202"/>
-      <c r="O15" s="202"/>
-      <c r="P15" s="202"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="196" t="s">
+      <c r="J15" s="196"/>
+      <c r="K15" s="196"/>
+      <c r="L15" s="196"/>
+      <c r="M15" s="196"/>
+      <c r="N15" s="197"/>
+      <c r="O15" s="197"/>
+      <c r="P15" s="197"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="194" t="s">
         <v>86</v>
       </c>
       <c r="B16" s="16"/>
@@ -5000,21 +4845,21 @@
       <c r="I16" s="52">
         <v>0.47699999999999998</v>
       </c>
-      <c r="J16" s="196" t="s">
+      <c r="J16" s="194" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="196" t="s">
+      <c r="K16" s="194" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="196" t="s">
+      <c r="L16" s="194" t="s">
         <v>27</v>
       </c>
-      <c r="M16" s="196" t="s">
+      <c r="M16" s="194" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="197"/>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="195"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="18">
@@ -5035,13 +4880,13 @@
       <c r="I17" s="53">
         <v>1</v>
       </c>
-      <c r="J17" s="197"/>
-      <c r="K17" s="197"/>
-      <c r="L17" s="197"/>
-      <c r="M17" s="197"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="197"/>
+      <c r="J17" s="195"/>
+      <c r="K17" s="195"/>
+      <c r="L17" s="195"/>
+      <c r="M17" s="195"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" s="195"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="18">
@@ -5062,13 +4907,13 @@
       <c r="I18" s="53">
         <v>1.45</v>
       </c>
-      <c r="J18" s="197"/>
-      <c r="K18" s="197"/>
-      <c r="L18" s="197"/>
-      <c r="M18" s="197"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="197"/>
+      <c r="J18" s="195"/>
+      <c r="K18" s="195"/>
+      <c r="L18" s="195"/>
+      <c r="M18" s="195"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" s="195"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="18">
@@ -5089,13 +4934,13 @@
       <c r="I19" s="53">
         <v>1.45</v>
       </c>
-      <c r="J19" s="197"/>
-      <c r="K19" s="197"/>
-      <c r="L19" s="197"/>
-      <c r="M19" s="197"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="197"/>
+      <c r="J19" s="195"/>
+      <c r="K19" s="195"/>
+      <c r="L19" s="195"/>
+      <c r="M19" s="195"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A20" s="195"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="18">
@@ -5116,13 +4961,13 @@
       <c r="I20" s="53">
         <v>1</v>
       </c>
-      <c r="J20" s="197"/>
-      <c r="K20" s="197"/>
-      <c r="L20" s="197"/>
-      <c r="M20" s="197"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="197"/>
+      <c r="J20" s="195"/>
+      <c r="K20" s="195"/>
+      <c r="L20" s="195"/>
+      <c r="M20" s="195"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21" s="195"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="18">
@@ -5148,8 +4993,8 @@
       <c r="L21" s="198"/>
       <c r="M21" s="198"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="196" t="s">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22" s="194" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="41"/>
@@ -5172,36 +5017,36 @@
       <c r="I22" s="65">
         <v>2</v>
       </c>
-      <c r="J22" s="196" t="s">
+      <c r="J22" s="194" t="s">
         <v>27</v>
       </c>
-      <c r="K22" s="196" t="s">
+      <c r="K22" s="194" t="s">
         <v>28</v>
       </c>
-      <c r="L22" s="196" t="s">
+      <c r="L22" s="194" t="s">
         <v>27</v>
       </c>
-      <c r="M22" s="196" t="s">
+      <c r="M22" s="194" t="s">
         <v>29</v>
       </c>
-      <c r="Q22" s="165">
+      <c r="Q22" s="163">
         <v>5</v>
       </c>
       <c r="R22" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="S22" s="165">
+      <c r="S22" s="163">
         <v>1.4</v>
       </c>
-      <c r="T22" s="165">
+      <c r="T22" s="163">
         <v>250</v>
       </c>
       <c r="U22" s="65">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="197"/>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23" s="195"/>
       <c r="B23" s="42"/>
       <c r="C23" s="53"/>
       <c r="D23" s="18">
@@ -5222,28 +5067,28 @@
       <c r="I23" s="65">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J23" s="197"/>
-      <c r="K23" s="197"/>
-      <c r="L23" s="197"/>
-      <c r="M23" s="197"/>
-      <c r="Q23" s="166">
+      <c r="J23" s="195"/>
+      <c r="K23" s="195"/>
+      <c r="L23" s="195"/>
+      <c r="M23" s="195"/>
+      <c r="Q23" s="164">
         <v>0.2</v>
       </c>
       <c r="R23" t="s">
         <v>34</v>
       </c>
-      <c r="S23" s="166">
+      <c r="S23" s="164">
         <v>0.35</v>
       </c>
-      <c r="T23" s="166">
+      <c r="T23" s="164">
         <v>900</v>
       </c>
       <c r="U23" s="65">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="197"/>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24" s="195"/>
       <c r="B24" s="53"/>
       <c r="C24" s="53"/>
       <c r="D24" s="18">
@@ -5264,28 +5109,28 @@
       <c r="I24" s="65">
         <v>2</v>
       </c>
-      <c r="J24" s="197"/>
-      <c r="K24" s="197"/>
-      <c r="L24" s="197"/>
-      <c r="M24" s="197"/>
-      <c r="Q24" s="166">
+      <c r="J24" s="195"/>
+      <c r="K24" s="195"/>
+      <c r="L24" s="195"/>
+      <c r="M24" s="195"/>
+      <c r="Q24" s="164">
         <v>5</v>
       </c>
       <c r="R24" t="s">
         <v>32</v>
       </c>
-      <c r="S24" s="166">
+      <c r="S24" s="164">
         <v>1.4</v>
       </c>
-      <c r="T24" s="166">
+      <c r="T24" s="164">
         <v>250</v>
       </c>
       <c r="U24" s="65">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="197"/>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A25" s="195"/>
       <c r="B25" s="53"/>
       <c r="C25" s="53"/>
       <c r="D25" s="18">
@@ -5306,28 +5151,28 @@
       <c r="I25" s="65">
         <v>0.77584580000000003</v>
       </c>
-      <c r="J25" s="197"/>
-      <c r="K25" s="197"/>
-      <c r="L25" s="197"/>
-      <c r="M25" s="197"/>
-      <c r="Q25" s="166">
+      <c r="J25" s="195"/>
+      <c r="K25" s="195"/>
+      <c r="L25" s="195"/>
+      <c r="M25" s="195"/>
+      <c r="Q25" s="164">
         <v>20</v>
       </c>
       <c r="R25" t="s">
         <v>74</v>
       </c>
-      <c r="S25" s="166">
+      <c r="S25" s="164">
         <v>1.94</v>
       </c>
-      <c r="T25" s="166">
+      <c r="T25" s="164">
         <v>2104.1999999999998</v>
       </c>
       <c r="U25" s="65">
         <v>0.77584580000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="197"/>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A26" s="195"/>
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
       <c r="D26" s="18">
@@ -5348,28 +5193,28 @@
       <c r="I26" s="54">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J26" s="197"/>
-      <c r="K26" s="197"/>
-      <c r="L26" s="197"/>
-      <c r="M26" s="197"/>
-      <c r="Q26" s="166">
+      <c r="J26" s="195"/>
+      <c r="K26" s="195"/>
+      <c r="L26" s="195"/>
+      <c r="M26" s="195"/>
+      <c r="Q26" s="164">
         <v>0.2</v>
       </c>
       <c r="R26" t="s">
         <v>34</v>
       </c>
-      <c r="S26" s="166">
+      <c r="S26" s="164">
         <v>0.35</v>
       </c>
-      <c r="T26" s="166">
+      <c r="T26" s="164">
         <v>900</v>
       </c>
-      <c r="U26" s="167">
+      <c r="U26" s="165">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="199"/>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A27" s="196"/>
       <c r="B27" s="44"/>
       <c r="C27" s="55"/>
       <c r="D27" s="13">
@@ -5390,28 +5235,28 @@
       <c r="I27" s="55">
         <v>1.38</v>
       </c>
-      <c r="J27" s="199"/>
-      <c r="K27" s="199"/>
-      <c r="L27" s="199"/>
-      <c r="M27" s="199"/>
-      <c r="Q27" s="168">
+      <c r="J27" s="196"/>
+      <c r="K27" s="196"/>
+      <c r="L27" s="196"/>
+      <c r="M27" s="196"/>
+      <c r="Q27" s="166">
         <v>10</v>
       </c>
       <c r="R27" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="S27" s="168">
+      <c r="S27" s="166">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="T27" s="168">
+      <c r="T27" s="166">
         <v>30</v>
       </c>
-      <c r="U27" s="168">
+      <c r="U27" s="166">
         <v>1.38</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="196" t="s">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A28" s="194" t="s">
         <v>96</v>
       </c>
       <c r="B28" s="76"/>
@@ -5424,13 +5269,13 @@
       <c r="G28" s="76"/>
       <c r="H28" s="76"/>
       <c r="I28" s="65"/>
-      <c r="J28" s="196"/>
-      <c r="K28" s="196"/>
-      <c r="L28" s="196"/>
-      <c r="M28" s="196"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="197"/>
+      <c r="J28" s="194"/>
+      <c r="K28" s="194"/>
+      <c r="L28" s="194"/>
+      <c r="M28" s="194"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A29" s="195"/>
       <c r="B29" s="77"/>
       <c r="C29" s="77"/>
       <c r="D29" s="18">
@@ -5441,13 +5286,13 @@
       <c r="G29" s="77"/>
       <c r="H29" s="77"/>
       <c r="I29" s="65"/>
-      <c r="J29" s="197"/>
-      <c r="K29" s="197"/>
-      <c r="L29" s="197"/>
-      <c r="M29" s="197"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="197"/>
+      <c r="J29" s="195"/>
+      <c r="K29" s="195"/>
+      <c r="L29" s="195"/>
+      <c r="M29" s="195"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A30" s="195"/>
       <c r="B30" s="77"/>
       <c r="C30" s="77"/>
       <c r="D30" s="18">
@@ -5458,13 +5303,13 @@
       <c r="G30" s="77"/>
       <c r="H30" s="77"/>
       <c r="I30" s="65"/>
-      <c r="J30" s="197"/>
-      <c r="K30" s="197"/>
-      <c r="L30" s="197"/>
-      <c r="M30" s="197"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="197"/>
+      <c r="J30" s="195"/>
+      <c r="K30" s="195"/>
+      <c r="L30" s="195"/>
+      <c r="M30" s="195"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A31" s="195"/>
       <c r="B31" s="77"/>
       <c r="C31" s="77"/>
       <c r="D31" s="18">
@@ -5475,13 +5320,13 @@
       <c r="G31" s="77"/>
       <c r="H31" s="77"/>
       <c r="I31" s="65"/>
-      <c r="J31" s="197"/>
-      <c r="K31" s="197"/>
-      <c r="L31" s="197"/>
-      <c r="M31" s="197"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="197"/>
+      <c r="J31" s="195"/>
+      <c r="K31" s="195"/>
+      <c r="L31" s="195"/>
+      <c r="M31" s="195"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A32" s="195"/>
       <c r="B32" s="77"/>
       <c r="C32" s="77"/>
       <c r="D32" s="18">
@@ -5492,13 +5337,13 @@
       <c r="G32" s="77"/>
       <c r="H32" s="77"/>
       <c r="I32" s="78"/>
-      <c r="J32" s="197"/>
-      <c r="K32" s="197"/>
-      <c r="L32" s="197"/>
-      <c r="M32" s="197"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="199"/>
+      <c r="J32" s="195"/>
+      <c r="K32" s="195"/>
+      <c r="L32" s="195"/>
+      <c r="M32" s="195"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="196"/>
       <c r="B33" s="79"/>
       <c r="C33" s="79"/>
       <c r="D33" s="13">
@@ -5509,13 +5354,13 @@
       <c r="G33" s="79"/>
       <c r="H33" s="79"/>
       <c r="I33" s="79"/>
-      <c r="J33" s="199"/>
-      <c r="K33" s="199"/>
-      <c r="L33" s="199"/>
-      <c r="M33" s="199"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="196" t="s">
+      <c r="J33" s="196"/>
+      <c r="K33" s="196"/>
+      <c r="L33" s="196"/>
+      <c r="M33" s="196"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="194" t="s">
         <v>95</v>
       </c>
       <c r="B34" s="76"/>
@@ -5528,13 +5373,13 @@
       <c r="G34" s="76"/>
       <c r="H34" s="76"/>
       <c r="I34" s="65"/>
-      <c r="J34" s="196"/>
-      <c r="K34" s="196"/>
-      <c r="L34" s="196"/>
-      <c r="M34" s="196"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="197"/>
+      <c r="J34" s="194"/>
+      <c r="K34" s="194"/>
+      <c r="L34" s="194"/>
+      <c r="M34" s="194"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="195"/>
       <c r="B35" s="77"/>
       <c r="C35" s="77"/>
       <c r="D35" s="18">
@@ -5545,13 +5390,13 @@
       <c r="G35" s="77"/>
       <c r="H35" s="77"/>
       <c r="I35" s="65"/>
-      <c r="J35" s="197"/>
-      <c r="K35" s="197"/>
-      <c r="L35" s="197"/>
-      <c r="M35" s="197"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="197"/>
+      <c r="J35" s="195"/>
+      <c r="K35" s="195"/>
+      <c r="L35" s="195"/>
+      <c r="M35" s="195"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="195"/>
       <c r="B36" s="77"/>
       <c r="C36" s="77"/>
       <c r="D36" s="18">
@@ -5562,13 +5407,13 @@
       <c r="G36" s="77"/>
       <c r="H36" s="77"/>
       <c r="I36" s="65"/>
-      <c r="J36" s="197"/>
-      <c r="K36" s="197"/>
-      <c r="L36" s="197"/>
-      <c r="M36" s="197"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="197"/>
+      <c r="J36" s="195"/>
+      <c r="K36" s="195"/>
+      <c r="L36" s="195"/>
+      <c r="M36" s="195"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="195"/>
       <c r="B37" s="77"/>
       <c r="C37" s="77"/>
       <c r="D37" s="18">
@@ -5579,13 +5424,13 @@
       <c r="G37" s="77"/>
       <c r="H37" s="77"/>
       <c r="I37" s="65"/>
-      <c r="J37" s="197"/>
-      <c r="K37" s="197"/>
-      <c r="L37" s="197"/>
-      <c r="M37" s="197"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="197"/>
+      <c r="J37" s="195"/>
+      <c r="K37" s="195"/>
+      <c r="L37" s="195"/>
+      <c r="M37" s="195"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="195"/>
       <c r="B38" s="77"/>
       <c r="C38" s="77"/>
       <c r="D38" s="18">
@@ -5596,13 +5441,13 @@
       <c r="G38" s="77"/>
       <c r="H38" s="77"/>
       <c r="I38" s="78"/>
-      <c r="J38" s="197"/>
-      <c r="K38" s="197"/>
-      <c r="L38" s="197"/>
-      <c r="M38" s="197"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="199"/>
+      <c r="J38" s="195"/>
+      <c r="K38" s="195"/>
+      <c r="L38" s="195"/>
+      <c r="M38" s="195"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="196"/>
       <c r="B39" s="79"/>
       <c r="C39" s="79"/>
       <c r="D39" s="13">
@@ -5613,12 +5458,12 @@
       <c r="G39" s="79"/>
       <c r="H39" s="79"/>
       <c r="I39" s="79"/>
-      <c r="J39" s="199"/>
-      <c r="K39" s="199"/>
-      <c r="L39" s="199"/>
-      <c r="M39" s="199"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J39" s="196"/>
+      <c r="K39" s="196"/>
+      <c r="L39" s="196"/>
+      <c r="M39" s="196"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="52" t="s">
         <v>109</v>
       </c>
@@ -5643,7 +5488,7 @@
       <c r="H40" s="71">
         <v>0</v>
       </c>
-      <c r="I40" s="148">
+      <c r="I40" s="146">
         <v>0</v>
       </c>
       <c r="J40" s="59" t="s">
@@ -5659,13 +5504,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="154" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="152" t="s">
         <v>72</v>
       </c>
       <c r="B41" s="71"/>
       <c r="C41" s="71"/>
-      <c r="D41" s="148">
+      <c r="D41" s="146">
         <v>0</v>
       </c>
       <c r="H41" s="71"/>
@@ -5675,127 +5520,125 @@
       <c r="L41" s="71"/>
       <c r="M41" s="71"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="196" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="194" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="150"/>
-      <c r="C42" s="150"/>
+      <c r="B42" s="148"/>
+      <c r="C42" s="148"/>
       <c r="D42" s="15">
         <v>0</v>
       </c>
-      <c r="E42" s="150"/>
+      <c r="E42" s="148"/>
       <c r="F42" s="16"/>
-      <c r="G42" s="150"/>
-      <c r="H42" s="150"/>
+      <c r="G42" s="148"/>
+      <c r="H42" s="148"/>
       <c r="I42" s="65"/>
-      <c r="J42" s="196"/>
-      <c r="K42" s="196"/>
-      <c r="L42" s="196"/>
-      <c r="M42" s="196"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="197"/>
-      <c r="B43" s="151"/>
-      <c r="C43" s="151"/>
+      <c r="J42" s="194"/>
+      <c r="K42" s="194"/>
+      <c r="L42" s="194"/>
+      <c r="M42" s="194"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="195"/>
+      <c r="B43" s="149"/>
+      <c r="C43" s="149"/>
       <c r="D43" s="18">
         <v>1</v>
       </c>
-      <c r="E43" s="151"/>
+      <c r="E43" s="149"/>
       <c r="F43"/>
-      <c r="G43" s="151"/>
-      <c r="H43" s="151"/>
+      <c r="G43" s="149"/>
+      <c r="H43" s="149"/>
       <c r="I43" s="65"/>
-      <c r="J43" s="197"/>
-      <c r="K43" s="197"/>
-      <c r="L43" s="197"/>
-      <c r="M43" s="197"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="197"/>
-      <c r="B44" s="151"/>
-      <c r="C44" s="151"/>
+      <c r="J43" s="195"/>
+      <c r="K43" s="195"/>
+      <c r="L43" s="195"/>
+      <c r="M43" s="195"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="195"/>
+      <c r="B44" s="149"/>
+      <c r="C44" s="149"/>
       <c r="D44" s="18">
         <v>2</v>
       </c>
-      <c r="E44" s="151"/>
+      <c r="E44" s="149"/>
       <c r="F44"/>
-      <c r="G44" s="151"/>
-      <c r="H44" s="151"/>
+      <c r="G44" s="149"/>
+      <c r="H44" s="149"/>
       <c r="I44" s="65"/>
-      <c r="J44" s="197"/>
-      <c r="K44" s="197"/>
-      <c r="L44" s="197"/>
-      <c r="M44" s="197"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="197"/>
-      <c r="B45" s="151"/>
-      <c r="C45" s="151"/>
+      <c r="J44" s="195"/>
+      <c r="K44" s="195"/>
+      <c r="L44" s="195"/>
+      <c r="M44" s="195"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="195"/>
+      <c r="B45" s="149"/>
+      <c r="C45" s="149"/>
       <c r="D45" s="18">
         <v>3</v>
       </c>
-      <c r="E45" s="151"/>
+      <c r="E45" s="149"/>
       <c r="F45"/>
-      <c r="G45" s="151"/>
-      <c r="H45" s="151"/>
+      <c r="G45" s="149"/>
+      <c r="H45" s="149"/>
       <c r="I45" s="65"/>
-      <c r="J45" s="197"/>
-      <c r="K45" s="197"/>
-      <c r="L45" s="197"/>
-      <c r="M45" s="197"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="197"/>
-      <c r="B46" s="151"/>
-      <c r="C46" s="151"/>
+      <c r="J45" s="195"/>
+      <c r="K45" s="195"/>
+      <c r="L45" s="195"/>
+      <c r="M45" s="195"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="195"/>
+      <c r="B46" s="149"/>
+      <c r="C46" s="149"/>
       <c r="D46" s="18">
         <v>4</v>
       </c>
-      <c r="E46" s="151"/>
+      <c r="E46" s="149"/>
       <c r="F46"/>
-      <c r="G46" s="151"/>
-      <c r="H46" s="151"/>
-      <c r="I46" s="153"/>
-      <c r="J46" s="197"/>
-      <c r="K46" s="197"/>
-      <c r="L46" s="197"/>
-      <c r="M46" s="197"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="199"/>
-      <c r="B47" s="152"/>
-      <c r="C47" s="152"/>
+      <c r="G46" s="149"/>
+      <c r="H46" s="149"/>
+      <c r="I46" s="151"/>
+      <c r="J46" s="195"/>
+      <c r="K46" s="195"/>
+      <c r="L46" s="195"/>
+      <c r="M46" s="195"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="196"/>
+      <c r="B47" s="150"/>
+      <c r="C47" s="150"/>
       <c r="D47" s="13">
         <v>5</v>
       </c>
-      <c r="E47" s="152"/>
+      <c r="E47" s="150"/>
       <c r="F47" s="14"/>
-      <c r="G47" s="152"/>
-      <c r="H47" s="152"/>
-      <c r="I47" s="152"/>
-      <c r="J47" s="199"/>
-      <c r="K47" s="199"/>
-      <c r="L47" s="199"/>
-      <c r="M47" s="199"/>
+      <c r="G47" s="150"/>
+      <c r="H47" s="150"/>
+      <c r="I47" s="150"/>
+      <c r="J47" s="196"/>
+      <c r="K47" s="196"/>
+      <c r="L47" s="196"/>
+      <c r="M47" s="196"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="J42:J47"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="M42:M47"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="J34:J39"/>
-    <mergeCell ref="K34:K39"/>
-    <mergeCell ref="L34:L39"/>
-    <mergeCell ref="M34:M39"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="J28:J33"/>
-    <mergeCell ref="K28:K33"/>
-    <mergeCell ref="L28:L33"/>
-    <mergeCell ref="M28:M33"/>
+    <mergeCell ref="L16:L21"/>
+    <mergeCell ref="M16:M21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="J22:J27"/>
+    <mergeCell ref="K22:K27"/>
+    <mergeCell ref="L22:L27"/>
+    <mergeCell ref="M22:M27"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="K16:K21"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="J16:J21"/>
     <mergeCell ref="N10:P15"/>
     <mergeCell ref="M10:M15"/>
     <mergeCell ref="J4:J9"/>
@@ -5805,19 +5648,21 @@
     <mergeCell ref="J10:J15"/>
     <mergeCell ref="K10:K15"/>
     <mergeCell ref="L10:L15"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="K16:K21"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="J16:J21"/>
-    <mergeCell ref="L16:L21"/>
-    <mergeCell ref="M16:M21"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="J22:J27"/>
-    <mergeCell ref="K22:K27"/>
-    <mergeCell ref="L22:L27"/>
-    <mergeCell ref="M22:M27"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="J28:J33"/>
+    <mergeCell ref="K28:K33"/>
+    <mergeCell ref="L28:L33"/>
+    <mergeCell ref="M28:M33"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="J34:J39"/>
+    <mergeCell ref="K34:K39"/>
+    <mergeCell ref="L34:L39"/>
+    <mergeCell ref="M34:M39"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="J42:J47"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="M42:M47"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>